<commit_message>
Fix: removing third section of blocks that are divided into 3
</commit_message>
<xml_diff>
--- a/data/residoodle_db.xlsx
+++ b/data/residoodle_db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackie.fortinflefil/PERSONAL/code/residoodle/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3589402E-2FEE-A74A-80E6-22E2B15876B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDB76B8-9C20-EA41-BF25-4C06F4AFDC51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{83F12362-36DA-4988-9448-F131A11196ED}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2598" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2598" uniqueCount="235">
   <si>
     <t>Resident</t>
   </si>
@@ -735,15 +735,9 @@
     <t>ED/US</t>
   </si>
   <si>
-    <t>US2/ED/LTJ</t>
-  </si>
-  <si>
     <t>CVICU/ED</t>
   </si>
   <si>
-    <t>CVICU/ED/Elec</t>
-  </si>
-  <si>
     <t>ED/CES</t>
   </si>
   <si>
@@ -756,16 +750,10 @@
     <t>CVICU/H Trauma</t>
   </si>
   <si>
-    <t>Elective/ED/HMC Trauma</t>
-  </si>
-  <si>
-    <t>ED/LTJ/CVICU</t>
-  </si>
-  <si>
     <t>EM/Elective</t>
   </si>
   <si>
-    <t>NA</t>
+    <t>ED/HMC Trauma</t>
   </si>
 </sst>
 </file>
@@ -1222,8 +1210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF91F7E-A94A-4218-9434-30BEAB935884}">
   <dimension ref="A1:E820"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A785" workbookViewId="0">
-      <selection activeCell="G805" sqref="G805"/>
+    <sheetView tabSelected="1" topLeftCell="A586" workbookViewId="0">
+      <selection activeCell="I605" sqref="I605"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1551,7 +1539,7 @@
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1570,7 +1558,7 @@
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1608,7 +1596,7 @@
         <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -2786,7 +2774,7 @@
         <v>6</v>
       </c>
       <c r="E82" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -5218,7 +5206,7 @@
         <v>4</v>
       </c>
       <c r="E210" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
@@ -5256,7 +5244,7 @@
         <v>6</v>
       </c>
       <c r="E212" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
@@ -5484,7 +5472,7 @@
         <v>5</v>
       </c>
       <c r="E224" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
@@ -5503,7 +5491,7 @@
         <v>6</v>
       </c>
       <c r="E225" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.2">
@@ -5617,7 +5605,7 @@
         <v>14</v>
       </c>
       <c r="E231" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
@@ -5788,7 +5776,7 @@
         <v>9</v>
       </c>
       <c r="E240" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.2">
@@ -5997,7 +5985,7 @@
         <v>6</v>
       </c>
       <c r="E251" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.2">
@@ -7004,7 +6992,7 @@
         <v>7</v>
       </c>
       <c r="E304" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.2">
@@ -7137,7 +7125,7 @@
         <v>16</v>
       </c>
       <c r="E311" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.2">
@@ -7194,7 +7182,7 @@
         <v>4</v>
       </c>
       <c r="E314" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.2">
@@ -7251,7 +7239,7 @@
         <v>7</v>
       </c>
       <c r="E317" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.2">
@@ -10405,7 +10393,7 @@
         <v>4</v>
       </c>
       <c r="E483" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="484" spans="1:5" x14ac:dyDescent="0.2">
@@ -10424,7 +10412,7 @@
         <v>5</v>
       </c>
       <c r="E484" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="485" spans="1:5" x14ac:dyDescent="0.2">
@@ -10443,7 +10431,7 @@
         <v>6</v>
       </c>
       <c r="E485" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="486" spans="1:5" x14ac:dyDescent="0.2">
@@ -10462,7 +10450,7 @@
         <v>7</v>
       </c>
       <c r="E486" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="487" spans="1:5" x14ac:dyDescent="0.2">
@@ -10481,7 +10469,7 @@
         <v>9</v>
       </c>
       <c r="E487" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="488" spans="1:5" x14ac:dyDescent="0.2">
@@ -10500,7 +10488,7 @@
         <v>11</v>
       </c>
       <c r="E488" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="489" spans="1:5" x14ac:dyDescent="0.2">
@@ -10519,7 +10507,7 @@
         <v>12</v>
       </c>
       <c r="E489" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="490" spans="1:5" x14ac:dyDescent="0.2">
@@ -10538,7 +10526,7 @@
         <v>13</v>
       </c>
       <c r="E490" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="491" spans="1:5" x14ac:dyDescent="0.2">
@@ -10557,7 +10545,7 @@
         <v>14</v>
       </c>
       <c r="E491" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="492" spans="1:5" x14ac:dyDescent="0.2">
@@ -10576,7 +10564,7 @@
         <v>15</v>
       </c>
       <c r="E492" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="493" spans="1:5" x14ac:dyDescent="0.2">
@@ -10595,7 +10583,7 @@
         <v>16</v>
       </c>
       <c r="E493" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="494" spans="1:5" x14ac:dyDescent="0.2">
@@ -10614,7 +10602,7 @@
         <v>17</v>
       </c>
       <c r="E494" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="495" spans="1:5" x14ac:dyDescent="0.2">
@@ -10633,7 +10621,7 @@
         <v>18</v>
       </c>
       <c r="E495" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="496" spans="1:5" x14ac:dyDescent="0.2">
@@ -12704,7 +12692,7 @@
         <v>9</v>
       </c>
       <c r="E604" t="s">
-        <v>228</v>
+        <v>35</v>
       </c>
     </row>
     <row r="605" spans="1:5" x14ac:dyDescent="0.2">
@@ -12875,7 +12863,7 @@
         <v>4</v>
       </c>
       <c r="E613" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="614" spans="1:5" x14ac:dyDescent="0.2">
@@ -12894,7 +12882,7 @@
         <v>5</v>
       </c>
       <c r="E614" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="615" spans="1:5" x14ac:dyDescent="0.2">
@@ -12913,7 +12901,7 @@
         <v>6</v>
       </c>
       <c r="E615" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="616" spans="1:5" x14ac:dyDescent="0.2">
@@ -12932,7 +12920,7 @@
         <v>7</v>
       </c>
       <c r="E616" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="617" spans="1:5" x14ac:dyDescent="0.2">
@@ -12951,7 +12939,7 @@
         <v>9</v>
       </c>
       <c r="E617" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="618" spans="1:5" x14ac:dyDescent="0.2">
@@ -12970,7 +12958,7 @@
         <v>11</v>
       </c>
       <c r="E618" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="619" spans="1:5" x14ac:dyDescent="0.2">
@@ -12989,7 +12977,7 @@
         <v>12</v>
       </c>
       <c r="E619" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="620" spans="1:5" x14ac:dyDescent="0.2">
@@ -13008,7 +12996,7 @@
         <v>13</v>
       </c>
       <c r="E620" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="621" spans="1:5" x14ac:dyDescent="0.2">
@@ -13027,7 +13015,7 @@
         <v>14</v>
       </c>
       <c r="E621" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="622" spans="1:5" x14ac:dyDescent="0.2">
@@ -13046,7 +13034,7 @@
         <v>15</v>
       </c>
       <c r="E622" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="623" spans="1:5" x14ac:dyDescent="0.2">
@@ -13065,7 +13053,7 @@
         <v>16</v>
       </c>
       <c r="E623" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="624" spans="1:5" x14ac:dyDescent="0.2">
@@ -13084,7 +13072,7 @@
         <v>17</v>
       </c>
       <c r="E624" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="625" spans="1:5" x14ac:dyDescent="0.2">
@@ -13103,7 +13091,7 @@
         <v>18</v>
       </c>
       <c r="E625" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="626" spans="1:5" x14ac:dyDescent="0.2">
@@ -13122,7 +13110,7 @@
         <v>4</v>
       </c>
       <c r="E626" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="627" spans="1:5" x14ac:dyDescent="0.2">
@@ -13141,7 +13129,7 @@
         <v>5</v>
       </c>
       <c r="E627" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="628" spans="1:5" x14ac:dyDescent="0.2">
@@ -13160,7 +13148,7 @@
         <v>6</v>
       </c>
       <c r="E628" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="629" spans="1:5" x14ac:dyDescent="0.2">
@@ -13179,7 +13167,7 @@
         <v>7</v>
       </c>
       <c r="E629" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="630" spans="1:5" x14ac:dyDescent="0.2">
@@ -13198,7 +13186,7 @@
         <v>9</v>
       </c>
       <c r="E630" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="631" spans="1:5" x14ac:dyDescent="0.2">
@@ -13217,7 +13205,7 @@
         <v>11</v>
       </c>
       <c r="E631" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="632" spans="1:5" x14ac:dyDescent="0.2">
@@ -13236,7 +13224,7 @@
         <v>12</v>
       </c>
       <c r="E632" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="633" spans="1:5" x14ac:dyDescent="0.2">
@@ -13255,7 +13243,7 @@
         <v>13</v>
       </c>
       <c r="E633" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="634" spans="1:5" x14ac:dyDescent="0.2">
@@ -13274,7 +13262,7 @@
         <v>14</v>
       </c>
       <c r="E634" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="635" spans="1:5" x14ac:dyDescent="0.2">
@@ -13293,7 +13281,7 @@
         <v>15</v>
       </c>
       <c r="E635" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="636" spans="1:5" x14ac:dyDescent="0.2">
@@ -13312,7 +13300,7 @@
         <v>16</v>
       </c>
       <c r="E636" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="637" spans="1:5" x14ac:dyDescent="0.2">
@@ -13331,7 +13319,7 @@
         <v>17</v>
       </c>
       <c r="E637" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="638" spans="1:5" x14ac:dyDescent="0.2">
@@ -13350,7 +13338,7 @@
         <v>18</v>
       </c>
       <c r="E638" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="639" spans="1:5" x14ac:dyDescent="0.2">
@@ -13369,7 +13357,7 @@
         <v>4</v>
       </c>
       <c r="E639" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="640" spans="1:5" x14ac:dyDescent="0.2">
@@ -13388,7 +13376,7 @@
         <v>5</v>
       </c>
       <c r="E640" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="641" spans="1:5" x14ac:dyDescent="0.2">
@@ -13407,7 +13395,7 @@
         <v>6</v>
       </c>
       <c r="E641" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="642" spans="1:5" x14ac:dyDescent="0.2">
@@ -13426,7 +13414,7 @@
         <v>7</v>
       </c>
       <c r="E642" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="643" spans="1:5" x14ac:dyDescent="0.2">
@@ -13445,7 +13433,7 @@
         <v>9</v>
       </c>
       <c r="E643" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="644" spans="1:5" x14ac:dyDescent="0.2">
@@ -13464,7 +13452,7 @@
         <v>11</v>
       </c>
       <c r="E644" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="645" spans="1:5" x14ac:dyDescent="0.2">
@@ -13483,7 +13471,7 @@
         <v>12</v>
       </c>
       <c r="E645" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="646" spans="1:5" x14ac:dyDescent="0.2">
@@ -13502,7 +13490,7 @@
         <v>13</v>
       </c>
       <c r="E646" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="647" spans="1:5" x14ac:dyDescent="0.2">
@@ -13521,7 +13509,7 @@
         <v>14</v>
       </c>
       <c r="E647" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="648" spans="1:5" x14ac:dyDescent="0.2">
@@ -13540,7 +13528,7 @@
         <v>15</v>
       </c>
       <c r="E648" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="649" spans="1:5" x14ac:dyDescent="0.2">
@@ -13559,7 +13547,7 @@
         <v>16</v>
       </c>
       <c r="E649" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="650" spans="1:5" x14ac:dyDescent="0.2">
@@ -13578,7 +13566,7 @@
         <v>17</v>
       </c>
       <c r="E650" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="651" spans="1:5" x14ac:dyDescent="0.2">
@@ -13597,7 +13585,7 @@
         <v>18</v>
       </c>
       <c r="E651" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="652" spans="1:5" x14ac:dyDescent="0.2">
@@ -13616,7 +13604,7 @@
         <v>4</v>
       </c>
       <c r="E652" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="653" spans="1:5" x14ac:dyDescent="0.2">
@@ -13635,7 +13623,7 @@
         <v>5</v>
       </c>
       <c r="E653" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="654" spans="1:5" x14ac:dyDescent="0.2">
@@ -13654,7 +13642,7 @@
         <v>6</v>
       </c>
       <c r="E654" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="655" spans="1:5" x14ac:dyDescent="0.2">
@@ -13673,7 +13661,7 @@
         <v>7</v>
       </c>
       <c r="E655" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="656" spans="1:5" x14ac:dyDescent="0.2">
@@ -13692,7 +13680,7 @@
         <v>9</v>
       </c>
       <c r="E656" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="657" spans="1:5" x14ac:dyDescent="0.2">
@@ -13711,7 +13699,7 @@
         <v>11</v>
       </c>
       <c r="E657" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="658" spans="1:5" x14ac:dyDescent="0.2">
@@ -13730,7 +13718,7 @@
         <v>12</v>
       </c>
       <c r="E658" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="659" spans="1:5" x14ac:dyDescent="0.2">
@@ -13749,7 +13737,7 @@
         <v>13</v>
       </c>
       <c r="E659" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="660" spans="1:5" x14ac:dyDescent="0.2">
@@ -13768,7 +13756,7 @@
         <v>14</v>
       </c>
       <c r="E660" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="661" spans="1:5" x14ac:dyDescent="0.2">
@@ -13787,7 +13775,7 @@
         <v>15</v>
       </c>
       <c r="E661" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="662" spans="1:5" x14ac:dyDescent="0.2">
@@ -13806,7 +13794,7 @@
         <v>16</v>
       </c>
       <c r="E662" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="663" spans="1:5" x14ac:dyDescent="0.2">
@@ -13825,7 +13813,7 @@
         <v>17</v>
       </c>
       <c r="E663" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="664" spans="1:5" x14ac:dyDescent="0.2">
@@ -13844,7 +13832,7 @@
         <v>18</v>
       </c>
       <c r="E664" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="665" spans="1:5" x14ac:dyDescent="0.2">
@@ -13863,7 +13851,7 @@
         <v>4</v>
       </c>
       <c r="E665" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="666" spans="1:5" x14ac:dyDescent="0.2">
@@ -13882,7 +13870,7 @@
         <v>5</v>
       </c>
       <c r="E666" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="667" spans="1:5" x14ac:dyDescent="0.2">
@@ -13901,7 +13889,7 @@
         <v>6</v>
       </c>
       <c r="E667" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="668" spans="1:5" x14ac:dyDescent="0.2">
@@ -13920,7 +13908,7 @@
         <v>7</v>
       </c>
       <c r="E668" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="669" spans="1:5" x14ac:dyDescent="0.2">
@@ -13939,7 +13927,7 @@
         <v>9</v>
       </c>
       <c r="E669" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="670" spans="1:5" x14ac:dyDescent="0.2">
@@ -13958,7 +13946,7 @@
         <v>11</v>
       </c>
       <c r="E670" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="671" spans="1:5" x14ac:dyDescent="0.2">
@@ -13977,7 +13965,7 @@
         <v>12</v>
       </c>
       <c r="E671" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="672" spans="1:5" x14ac:dyDescent="0.2">
@@ -13996,7 +13984,7 @@
         <v>13</v>
       </c>
       <c r="E672" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="673" spans="1:5" x14ac:dyDescent="0.2">
@@ -14015,7 +14003,7 @@
         <v>14</v>
       </c>
       <c r="E673" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="674" spans="1:5" x14ac:dyDescent="0.2">
@@ -14034,7 +14022,7 @@
         <v>15</v>
       </c>
       <c r="E674" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="675" spans="1:5" x14ac:dyDescent="0.2">
@@ -14053,7 +14041,7 @@
         <v>16</v>
       </c>
       <c r="E675" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="676" spans="1:5" x14ac:dyDescent="0.2">
@@ -14072,7 +14060,7 @@
         <v>17</v>
       </c>
       <c r="E676" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="677" spans="1:5" x14ac:dyDescent="0.2">
@@ -14091,7 +14079,7 @@
         <v>18</v>
       </c>
       <c r="E677" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="678" spans="1:5" x14ac:dyDescent="0.2">
@@ -14110,7 +14098,7 @@
         <v>4</v>
       </c>
       <c r="E678" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="679" spans="1:5" x14ac:dyDescent="0.2">
@@ -14129,7 +14117,7 @@
         <v>5</v>
       </c>
       <c r="E679" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="680" spans="1:5" x14ac:dyDescent="0.2">
@@ -14148,7 +14136,7 @@
         <v>6</v>
       </c>
       <c r="E680" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="681" spans="1:5" x14ac:dyDescent="0.2">
@@ -14167,7 +14155,7 @@
         <v>7</v>
       </c>
       <c r="E681" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="682" spans="1:5" x14ac:dyDescent="0.2">
@@ -14186,7 +14174,7 @@
         <v>9</v>
       </c>
       <c r="E682" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="683" spans="1:5" x14ac:dyDescent="0.2">
@@ -14205,7 +14193,7 @@
         <v>11</v>
       </c>
       <c r="E683" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="684" spans="1:5" x14ac:dyDescent="0.2">
@@ -14224,7 +14212,7 @@
         <v>12</v>
       </c>
       <c r="E684" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="685" spans="1:5" x14ac:dyDescent="0.2">
@@ -14243,7 +14231,7 @@
         <v>13</v>
       </c>
       <c r="E685" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="686" spans="1:5" x14ac:dyDescent="0.2">
@@ -14262,7 +14250,7 @@
         <v>14</v>
       </c>
       <c r="E686" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="687" spans="1:5" x14ac:dyDescent="0.2">
@@ -14281,7 +14269,7 @@
         <v>15</v>
       </c>
       <c r="E687" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="688" spans="1:5" x14ac:dyDescent="0.2">
@@ -14300,7 +14288,7 @@
         <v>16</v>
       </c>
       <c r="E688" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="689" spans="1:5" x14ac:dyDescent="0.2">
@@ -14319,7 +14307,7 @@
         <v>17</v>
       </c>
       <c r="E689" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="690" spans="1:5" x14ac:dyDescent="0.2">
@@ -14338,7 +14326,7 @@
         <v>18</v>
       </c>
       <c r="E690" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="691" spans="1:5" x14ac:dyDescent="0.2">
@@ -14357,7 +14345,7 @@
         <v>4</v>
       </c>
       <c r="E691" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="692" spans="1:5" x14ac:dyDescent="0.2">
@@ -14376,7 +14364,7 @@
         <v>5</v>
       </c>
       <c r="E692" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="693" spans="1:5" x14ac:dyDescent="0.2">
@@ -14395,7 +14383,7 @@
         <v>6</v>
       </c>
       <c r="E693" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="694" spans="1:5" x14ac:dyDescent="0.2">
@@ -14414,7 +14402,7 @@
         <v>7</v>
       </c>
       <c r="E694" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="695" spans="1:5" x14ac:dyDescent="0.2">
@@ -14433,7 +14421,7 @@
         <v>9</v>
       </c>
       <c r="E695" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="696" spans="1:5" x14ac:dyDescent="0.2">
@@ -14452,7 +14440,7 @@
         <v>11</v>
       </c>
       <c r="E696" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="697" spans="1:5" x14ac:dyDescent="0.2">
@@ -14471,7 +14459,7 @@
         <v>12</v>
       </c>
       <c r="E697" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="698" spans="1:5" x14ac:dyDescent="0.2">
@@ -14490,7 +14478,7 @@
         <v>13</v>
       </c>
       <c r="E698" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="699" spans="1:5" x14ac:dyDescent="0.2">
@@ -14509,7 +14497,7 @@
         <v>14</v>
       </c>
       <c r="E699" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="700" spans="1:5" x14ac:dyDescent="0.2">
@@ -14528,7 +14516,7 @@
         <v>15</v>
       </c>
       <c r="E700" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="701" spans="1:5" x14ac:dyDescent="0.2">
@@ -14547,7 +14535,7 @@
         <v>16</v>
       </c>
       <c r="E701" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="702" spans="1:5" x14ac:dyDescent="0.2">
@@ -14566,7 +14554,7 @@
         <v>17</v>
       </c>
       <c r="E702" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="703" spans="1:5" x14ac:dyDescent="0.2">
@@ -14585,7 +14573,7 @@
         <v>18</v>
       </c>
       <c r="E703" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="704" spans="1:5" x14ac:dyDescent="0.2">
@@ -14604,7 +14592,7 @@
         <v>4</v>
       </c>
       <c r="E704" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="705" spans="1:5" x14ac:dyDescent="0.2">
@@ -14623,7 +14611,7 @@
         <v>5</v>
       </c>
       <c r="E705" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="706" spans="1:5" x14ac:dyDescent="0.2">
@@ -14642,7 +14630,7 @@
         <v>6</v>
       </c>
       <c r="E706" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="707" spans="1:5" x14ac:dyDescent="0.2">
@@ -14661,7 +14649,7 @@
         <v>7</v>
       </c>
       <c r="E707" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="708" spans="1:5" x14ac:dyDescent="0.2">
@@ -14680,7 +14668,7 @@
         <v>9</v>
       </c>
       <c r="E708" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="709" spans="1:5" x14ac:dyDescent="0.2">
@@ -14699,7 +14687,7 @@
         <v>11</v>
       </c>
       <c r="E709" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="710" spans="1:5" x14ac:dyDescent="0.2">
@@ -14718,7 +14706,7 @@
         <v>12</v>
       </c>
       <c r="E710" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="711" spans="1:5" x14ac:dyDescent="0.2">
@@ -14737,7 +14725,7 @@
         <v>13</v>
       </c>
       <c r="E711" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="712" spans="1:5" x14ac:dyDescent="0.2">
@@ -14756,7 +14744,7 @@
         <v>14</v>
       </c>
       <c r="E712" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="713" spans="1:5" x14ac:dyDescent="0.2">
@@ -14775,7 +14763,7 @@
         <v>15</v>
       </c>
       <c r="E713" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="714" spans="1:5" x14ac:dyDescent="0.2">
@@ -14794,7 +14782,7 @@
         <v>16</v>
       </c>
       <c r="E714" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="715" spans="1:5" x14ac:dyDescent="0.2">
@@ -14813,7 +14801,7 @@
         <v>17</v>
       </c>
       <c r="E715" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="716" spans="1:5" x14ac:dyDescent="0.2">
@@ -14832,7 +14820,7 @@
         <v>18</v>
       </c>
       <c r="E716" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="717" spans="1:5" x14ac:dyDescent="0.2">
@@ -14851,7 +14839,7 @@
         <v>4</v>
       </c>
       <c r="E717" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="718" spans="1:5" x14ac:dyDescent="0.2">
@@ -14870,7 +14858,7 @@
         <v>5</v>
       </c>
       <c r="E718" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="719" spans="1:5" x14ac:dyDescent="0.2">
@@ -14889,7 +14877,7 @@
         <v>6</v>
       </c>
       <c r="E719" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="720" spans="1:5" x14ac:dyDescent="0.2">
@@ -14908,7 +14896,7 @@
         <v>7</v>
       </c>
       <c r="E720" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="721" spans="1:5" x14ac:dyDescent="0.2">
@@ -14927,7 +14915,7 @@
         <v>9</v>
       </c>
       <c r="E721" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="722" spans="1:5" x14ac:dyDescent="0.2">
@@ -14946,7 +14934,7 @@
         <v>11</v>
       </c>
       <c r="E722" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="723" spans="1:5" x14ac:dyDescent="0.2">
@@ -14965,7 +14953,7 @@
         <v>12</v>
       </c>
       <c r="E723" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="724" spans="1:5" x14ac:dyDescent="0.2">
@@ -14984,7 +14972,7 @@
         <v>13</v>
       </c>
       <c r="E724" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="725" spans="1:5" x14ac:dyDescent="0.2">
@@ -15003,7 +14991,7 @@
         <v>14</v>
       </c>
       <c r="E725" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="726" spans="1:5" x14ac:dyDescent="0.2">
@@ -15022,7 +15010,7 @@
         <v>15</v>
       </c>
       <c r="E726" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="727" spans="1:5" x14ac:dyDescent="0.2">
@@ -15041,7 +15029,7 @@
         <v>16</v>
       </c>
       <c r="E727" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="728" spans="1:5" x14ac:dyDescent="0.2">
@@ -15060,7 +15048,7 @@
         <v>17</v>
       </c>
       <c r="E728" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="729" spans="1:5" x14ac:dyDescent="0.2">
@@ -15079,7 +15067,7 @@
         <v>18</v>
       </c>
       <c r="E729" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="730" spans="1:5" x14ac:dyDescent="0.2">
@@ -15098,7 +15086,7 @@
         <v>4</v>
       </c>
       <c r="E730" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="731" spans="1:5" x14ac:dyDescent="0.2">
@@ -15117,7 +15105,7 @@
         <v>5</v>
       </c>
       <c r="E731" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="732" spans="1:5" x14ac:dyDescent="0.2">
@@ -15136,7 +15124,7 @@
         <v>6</v>
       </c>
       <c r="E732" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="733" spans="1:5" x14ac:dyDescent="0.2">
@@ -15155,7 +15143,7 @@
         <v>7</v>
       </c>
       <c r="E733" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="734" spans="1:5" x14ac:dyDescent="0.2">
@@ -15174,7 +15162,7 @@
         <v>9</v>
       </c>
       <c r="E734" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="735" spans="1:5" x14ac:dyDescent="0.2">
@@ -15193,7 +15181,7 @@
         <v>11</v>
       </c>
       <c r="E735" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="736" spans="1:5" x14ac:dyDescent="0.2">
@@ -15212,7 +15200,7 @@
         <v>12</v>
       </c>
       <c r="E736" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="737" spans="1:5" x14ac:dyDescent="0.2">
@@ -15231,7 +15219,7 @@
         <v>13</v>
       </c>
       <c r="E737" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="738" spans="1:5" x14ac:dyDescent="0.2">
@@ -15250,7 +15238,7 @@
         <v>14</v>
       </c>
       <c r="E738" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="739" spans="1:5" x14ac:dyDescent="0.2">
@@ -15269,7 +15257,7 @@
         <v>15</v>
       </c>
       <c r="E739" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="740" spans="1:5" x14ac:dyDescent="0.2">
@@ -15288,7 +15276,7 @@
         <v>16</v>
       </c>
       <c r="E740" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="741" spans="1:5" x14ac:dyDescent="0.2">
@@ -15307,7 +15295,7 @@
         <v>17</v>
       </c>
       <c r="E741" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="742" spans="1:5" x14ac:dyDescent="0.2">
@@ -15326,7 +15314,7 @@
         <v>18</v>
       </c>
       <c r="E742" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="743" spans="1:5" x14ac:dyDescent="0.2">
@@ -15345,7 +15333,7 @@
         <v>4</v>
       </c>
       <c r="E743" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="744" spans="1:5" x14ac:dyDescent="0.2">
@@ -15364,7 +15352,7 @@
         <v>5</v>
       </c>
       <c r="E744" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="745" spans="1:5" x14ac:dyDescent="0.2">
@@ -15383,7 +15371,7 @@
         <v>6</v>
       </c>
       <c r="E745" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="746" spans="1:5" x14ac:dyDescent="0.2">
@@ -15402,7 +15390,7 @@
         <v>7</v>
       </c>
       <c r="E746" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="747" spans="1:5" x14ac:dyDescent="0.2">
@@ -15421,7 +15409,7 @@
         <v>9</v>
       </c>
       <c r="E747" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="748" spans="1:5" x14ac:dyDescent="0.2">
@@ -15440,7 +15428,7 @@
         <v>11</v>
       </c>
       <c r="E748" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="749" spans="1:5" x14ac:dyDescent="0.2">
@@ -15459,7 +15447,7 @@
         <v>12</v>
       </c>
       <c r="E749" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="750" spans="1:5" x14ac:dyDescent="0.2">
@@ -15478,7 +15466,7 @@
         <v>13</v>
       </c>
       <c r="E750" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="751" spans="1:5" x14ac:dyDescent="0.2">
@@ -15497,7 +15485,7 @@
         <v>14</v>
       </c>
       <c r="E751" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="752" spans="1:5" x14ac:dyDescent="0.2">
@@ -15516,7 +15504,7 @@
         <v>15</v>
       </c>
       <c r="E752" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="753" spans="1:5" x14ac:dyDescent="0.2">
@@ -15535,7 +15523,7 @@
         <v>16</v>
       </c>
       <c r="E753" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="754" spans="1:5" x14ac:dyDescent="0.2">
@@ -15554,7 +15542,7 @@
         <v>17</v>
       </c>
       <c r="E754" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="755" spans="1:5" x14ac:dyDescent="0.2">
@@ -15573,7 +15561,7 @@
         <v>18</v>
       </c>
       <c r="E755" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="756" spans="1:5" x14ac:dyDescent="0.2">
@@ -15592,7 +15580,7 @@
         <v>4</v>
       </c>
       <c r="E756" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="757" spans="1:5" x14ac:dyDescent="0.2">
@@ -15611,7 +15599,7 @@
         <v>5</v>
       </c>
       <c r="E757" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="758" spans="1:5" x14ac:dyDescent="0.2">
@@ -15630,7 +15618,7 @@
         <v>6</v>
       </c>
       <c r="E758" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="759" spans="1:5" x14ac:dyDescent="0.2">
@@ -15649,7 +15637,7 @@
         <v>7</v>
       </c>
       <c r="E759" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="760" spans="1:5" x14ac:dyDescent="0.2">
@@ -15668,7 +15656,7 @@
         <v>9</v>
       </c>
       <c r="E760" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="761" spans="1:5" x14ac:dyDescent="0.2">
@@ -15687,7 +15675,7 @@
         <v>11</v>
       </c>
       <c r="E761" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="762" spans="1:5" x14ac:dyDescent="0.2">
@@ -15706,7 +15694,7 @@
         <v>12</v>
       </c>
       <c r="E762" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="763" spans="1:5" x14ac:dyDescent="0.2">
@@ -15725,7 +15713,7 @@
         <v>13</v>
       </c>
       <c r="E763" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="764" spans="1:5" x14ac:dyDescent="0.2">
@@ -15744,7 +15732,7 @@
         <v>14</v>
       </c>
       <c r="E764" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="765" spans="1:5" x14ac:dyDescent="0.2">
@@ -15763,7 +15751,7 @@
         <v>15</v>
       </c>
       <c r="E765" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="766" spans="1:5" x14ac:dyDescent="0.2">
@@ -15782,7 +15770,7 @@
         <v>16</v>
       </c>
       <c r="E766" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="767" spans="1:5" x14ac:dyDescent="0.2">
@@ -15801,7 +15789,7 @@
         <v>17</v>
       </c>
       <c r="E767" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="768" spans="1:5" x14ac:dyDescent="0.2">
@@ -15820,7 +15808,7 @@
         <v>18</v>
       </c>
       <c r="E768" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="769" spans="1:5" x14ac:dyDescent="0.2">
@@ -15839,7 +15827,7 @@
         <v>4</v>
       </c>
       <c r="E769" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="770" spans="1:5" x14ac:dyDescent="0.2">
@@ -15858,7 +15846,7 @@
         <v>5</v>
       </c>
       <c r="E770" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="771" spans="1:5" x14ac:dyDescent="0.2">
@@ -15877,7 +15865,7 @@
         <v>6</v>
       </c>
       <c r="E771" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="772" spans="1:5" x14ac:dyDescent="0.2">
@@ -15896,7 +15884,7 @@
         <v>7</v>
       </c>
       <c r="E772" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="773" spans="1:5" x14ac:dyDescent="0.2">
@@ -15915,7 +15903,7 @@
         <v>9</v>
       </c>
       <c r="E773" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="774" spans="1:5" x14ac:dyDescent="0.2">
@@ -15934,7 +15922,7 @@
         <v>11</v>
       </c>
       <c r="E774" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="775" spans="1:5" x14ac:dyDescent="0.2">
@@ -15953,7 +15941,7 @@
         <v>12</v>
       </c>
       <c r="E775" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="776" spans="1:5" x14ac:dyDescent="0.2">
@@ -15972,7 +15960,7 @@
         <v>13</v>
       </c>
       <c r="E776" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="777" spans="1:5" x14ac:dyDescent="0.2">
@@ -15991,7 +15979,7 @@
         <v>14</v>
       </c>
       <c r="E777" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="778" spans="1:5" x14ac:dyDescent="0.2">
@@ -16010,7 +15998,7 @@
         <v>15</v>
       </c>
       <c r="E778" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="779" spans="1:5" x14ac:dyDescent="0.2">
@@ -16029,7 +16017,7 @@
         <v>16</v>
       </c>
       <c r="E779" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="780" spans="1:5" x14ac:dyDescent="0.2">
@@ -16048,7 +16036,7 @@
         <v>17</v>
       </c>
       <c r="E780" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="781" spans="1:5" x14ac:dyDescent="0.2">
@@ -16067,7 +16055,7 @@
         <v>18</v>
       </c>
       <c r="E781" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="782" spans="1:5" x14ac:dyDescent="0.2">
@@ -16086,7 +16074,7 @@
         <v>4</v>
       </c>
       <c r="E782" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="783" spans="1:5" x14ac:dyDescent="0.2">
@@ -16105,7 +16093,7 @@
         <v>5</v>
       </c>
       <c r="E783" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="784" spans="1:5" x14ac:dyDescent="0.2">
@@ -16124,7 +16112,7 @@
         <v>6</v>
       </c>
       <c r="E784" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="785" spans="1:5" x14ac:dyDescent="0.2">
@@ -16143,7 +16131,7 @@
         <v>7</v>
       </c>
       <c r="E785" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="786" spans="1:5" x14ac:dyDescent="0.2">
@@ -16162,7 +16150,7 @@
         <v>9</v>
       </c>
       <c r="E786" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="787" spans="1:5" x14ac:dyDescent="0.2">
@@ -16181,7 +16169,7 @@
         <v>11</v>
       </c>
       <c r="E787" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="788" spans="1:5" x14ac:dyDescent="0.2">
@@ -16200,7 +16188,7 @@
         <v>12</v>
       </c>
       <c r="E788" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="789" spans="1:5" x14ac:dyDescent="0.2">
@@ -16219,7 +16207,7 @@
         <v>13</v>
       </c>
       <c r="E789" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="790" spans="1:5" x14ac:dyDescent="0.2">
@@ -16238,7 +16226,7 @@
         <v>14</v>
       </c>
       <c r="E790" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="791" spans="1:5" x14ac:dyDescent="0.2">
@@ -16257,7 +16245,7 @@
         <v>15</v>
       </c>
       <c r="E791" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="792" spans="1:5" x14ac:dyDescent="0.2">
@@ -16276,7 +16264,7 @@
         <v>16</v>
       </c>
       <c r="E792" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="793" spans="1:5" x14ac:dyDescent="0.2">
@@ -16295,7 +16283,7 @@
         <v>17</v>
       </c>
       <c r="E793" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="794" spans="1:5" x14ac:dyDescent="0.2">
@@ -16314,7 +16302,7 @@
         <v>18</v>
       </c>
       <c r="E794" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="795" spans="1:5" x14ac:dyDescent="0.2">
@@ -16333,7 +16321,7 @@
         <v>4</v>
       </c>
       <c r="E795" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="796" spans="1:5" x14ac:dyDescent="0.2">
@@ -16352,7 +16340,7 @@
         <v>5</v>
       </c>
       <c r="E796" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="797" spans="1:5" x14ac:dyDescent="0.2">
@@ -16371,7 +16359,7 @@
         <v>6</v>
       </c>
       <c r="E797" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="798" spans="1:5" x14ac:dyDescent="0.2">
@@ -16390,7 +16378,7 @@
         <v>7</v>
       </c>
       <c r="E798" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="799" spans="1:5" x14ac:dyDescent="0.2">
@@ -16409,7 +16397,7 @@
         <v>9</v>
       </c>
       <c r="E799" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="800" spans="1:5" x14ac:dyDescent="0.2">
@@ -16428,7 +16416,7 @@
         <v>11</v>
       </c>
       <c r="E800" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="801" spans="1:5" x14ac:dyDescent="0.2">
@@ -16447,7 +16435,7 @@
         <v>12</v>
       </c>
       <c r="E801" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="802" spans="1:5" x14ac:dyDescent="0.2">
@@ -16466,7 +16454,7 @@
         <v>13</v>
       </c>
       <c r="E802" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="803" spans="1:5" x14ac:dyDescent="0.2">
@@ -16485,7 +16473,7 @@
         <v>14</v>
       </c>
       <c r="E803" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="804" spans="1:5" x14ac:dyDescent="0.2">
@@ -16504,7 +16492,7 @@
         <v>15</v>
       </c>
       <c r="E804" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="805" spans="1:5" x14ac:dyDescent="0.2">
@@ -16523,7 +16511,7 @@
         <v>16</v>
       </c>
       <c r="E805" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="806" spans="1:5" x14ac:dyDescent="0.2">
@@ -16542,7 +16530,7 @@
         <v>17</v>
       </c>
       <c r="E806" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="807" spans="1:5" x14ac:dyDescent="0.2">
@@ -16561,7 +16549,7 @@
         <v>18</v>
       </c>
       <c r="E807" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="808" spans="1:5" x14ac:dyDescent="0.2">
@@ -16580,7 +16568,7 @@
         <v>4</v>
       </c>
       <c r="E808" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="809" spans="1:5" x14ac:dyDescent="0.2">
@@ -16599,7 +16587,7 @@
         <v>5</v>
       </c>
       <c r="E809" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="810" spans="1:5" x14ac:dyDescent="0.2">
@@ -16618,7 +16606,7 @@
         <v>6</v>
       </c>
       <c r="E810" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="811" spans="1:5" x14ac:dyDescent="0.2">
@@ -16637,7 +16625,7 @@
         <v>7</v>
       </c>
       <c r="E811" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="812" spans="1:5" x14ac:dyDescent="0.2">
@@ -16656,7 +16644,7 @@
         <v>9</v>
       </c>
       <c r="E812" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="813" spans="1:5" x14ac:dyDescent="0.2">
@@ -16675,7 +16663,7 @@
         <v>11</v>
       </c>
       <c r="E813" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="814" spans="1:5" x14ac:dyDescent="0.2">
@@ -16694,7 +16682,7 @@
         <v>12</v>
       </c>
       <c r="E814" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="815" spans="1:5" x14ac:dyDescent="0.2">
@@ -16713,7 +16701,7 @@
         <v>13</v>
       </c>
       <c r="E815" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="816" spans="1:5" x14ac:dyDescent="0.2">
@@ -16732,7 +16720,7 @@
         <v>14</v>
       </c>
       <c r="E816" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="817" spans="1:5" x14ac:dyDescent="0.2">
@@ -16751,7 +16739,7 @@
         <v>15</v>
       </c>
       <c r="E817" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="818" spans="1:5" x14ac:dyDescent="0.2">
@@ -16770,7 +16758,7 @@
         <v>16</v>
       </c>
       <c r="E818" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="819" spans="1:5" x14ac:dyDescent="0.2">
@@ -16789,7 +16777,7 @@
         <v>17</v>
       </c>
       <c r="E819" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
     <row r="820" spans="1:5" x14ac:dyDescent="0.2">
@@ -16808,7 +16796,7 @@
         <v>18</v>
       </c>
       <c r="E820" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -17043,8 +17031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5CC31C-6869-47E7-A440-832340BE0ED2}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix: updating user IDs
</commit_message>
<xml_diff>
--- a/data/residoodle_db.xlsx
+++ b/data/residoodle_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackie.fortinflefil/PERSONAL/code/residoodle/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A98FBF-4D67-9A4E-9FD7-1697C03259D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C2BA9B-62AE-3C47-BBDF-897BC870CE5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{83F12362-36DA-4988-9448-F131A11196ED}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" activeTab="2" xr2:uid="{83F12362-36DA-4988-9448-F131A11196ED}"/>
   </bookViews>
   <sheets>
     <sheet name="ResidentBlockSchedule" sheetId="1" r:id="rId1"/>
@@ -1230,8 +1230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF91F7E-A94A-4218-9434-30BEAB935884}">
   <dimension ref="A1:E820"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A750" workbookViewId="0">
+      <selection activeCell="E819" sqref="E819"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12383,7 +12383,7 @@
       </c>
       <c r="C587">
         <f>INDEX(Residents[], MATCH(B587,Residents[fullName], 0), 1)</f>
-        <v>2804</v>
+        <v>3072</v>
       </c>
       <c r="D587" t="s">
         <v>4</v>
@@ -12402,7 +12402,7 @@
       </c>
       <c r="C588">
         <f>INDEX(Residents[], MATCH(B588,Residents[fullName], 0), 1)</f>
-        <v>2804</v>
+        <v>3072</v>
       </c>
       <c r="D588" t="s">
         <v>5</v>
@@ -12421,7 +12421,7 @@
       </c>
       <c r="C589">
         <f>INDEX(Residents[], MATCH(B589,Residents[fullName], 0), 1)</f>
-        <v>2804</v>
+        <v>3072</v>
       </c>
       <c r="D589" t="s">
         <v>6</v>
@@ -12440,7 +12440,7 @@
       </c>
       <c r="C590">
         <f>INDEX(Residents[], MATCH(B590,Residents[fullName], 0), 1)</f>
-        <v>2804</v>
+        <v>3072</v>
       </c>
       <c r="D590" t="s">
         <v>7</v>
@@ -12459,7 +12459,7 @@
       </c>
       <c r="C591">
         <f>INDEX(Residents[], MATCH(B591,Residents[fullName], 0), 1)</f>
-        <v>2804</v>
+        <v>3072</v>
       </c>
       <c r="D591" t="s">
         <v>9</v>
@@ -12478,7 +12478,7 @@
       </c>
       <c r="C592">
         <f>INDEX(Residents[], MATCH(B592,Residents[fullName], 0), 1)</f>
-        <v>2804</v>
+        <v>3072</v>
       </c>
       <c r="D592" t="s">
         <v>11</v>
@@ -12497,7 +12497,7 @@
       </c>
       <c r="C593">
         <f>INDEX(Residents[], MATCH(B593,Residents[fullName], 0), 1)</f>
-        <v>2804</v>
+        <v>3072</v>
       </c>
       <c r="D593" t="s">
         <v>12</v>
@@ -12516,7 +12516,7 @@
       </c>
       <c r="C594">
         <f>INDEX(Residents[], MATCH(B594,Residents[fullName], 0), 1)</f>
-        <v>2804</v>
+        <v>3072</v>
       </c>
       <c r="D594" t="s">
         <v>13</v>
@@ -12535,7 +12535,7 @@
       </c>
       <c r="C595">
         <f>INDEX(Residents[], MATCH(B595,Residents[fullName], 0), 1)</f>
-        <v>2804</v>
+        <v>3072</v>
       </c>
       <c r="D595" t="s">
         <v>14</v>
@@ -12554,7 +12554,7 @@
       </c>
       <c r="C596">
         <f>INDEX(Residents[], MATCH(B596,Residents[fullName], 0), 1)</f>
-        <v>2804</v>
+        <v>3072</v>
       </c>
       <c r="D596" t="s">
         <v>15</v>
@@ -12573,7 +12573,7 @@
       </c>
       <c r="C597">
         <f>INDEX(Residents[], MATCH(B597,Residents[fullName], 0), 1)</f>
-        <v>2804</v>
+        <v>3072</v>
       </c>
       <c r="D597" t="s">
         <v>16</v>
@@ -12592,7 +12592,7 @@
       </c>
       <c r="C598">
         <f>INDEX(Residents[], MATCH(B598,Residents[fullName], 0), 1)</f>
-        <v>2804</v>
+        <v>3072</v>
       </c>
       <c r="D598" t="s">
         <v>17</v>
@@ -12611,7 +12611,7 @@
       </c>
       <c r="C599">
         <f>INDEX(Residents[], MATCH(B599,Residents[fullName], 0), 1)</f>
-        <v>2804</v>
+        <v>3072</v>
       </c>
       <c r="D599" t="s">
         <v>18</v>
@@ -12630,7 +12630,7 @@
       </c>
       <c r="C600">
         <f>INDEX(Residents[], MATCH(B600,Residents[fullName], 0), 1)</f>
-        <v>2805</v>
+        <v>3073</v>
       </c>
       <c r="D600" t="s">
         <v>4</v>
@@ -12649,7 +12649,7 @@
       </c>
       <c r="C601">
         <f>INDEX(Residents[], MATCH(B601,Residents[fullName], 0), 1)</f>
-        <v>2805</v>
+        <v>3073</v>
       </c>
       <c r="D601" t="s">
         <v>5</v>
@@ -12668,7 +12668,7 @@
       </c>
       <c r="C602">
         <f>INDEX(Residents[], MATCH(B602,Residents[fullName], 0), 1)</f>
-        <v>2805</v>
+        <v>3073</v>
       </c>
       <c r="D602" t="s">
         <v>6</v>
@@ -12687,7 +12687,7 @@
       </c>
       <c r="C603">
         <f>INDEX(Residents[], MATCH(B603,Residents[fullName], 0), 1)</f>
-        <v>2805</v>
+        <v>3073</v>
       </c>
       <c r="D603" t="s">
         <v>7</v>
@@ -12706,7 +12706,7 @@
       </c>
       <c r="C604">
         <f>INDEX(Residents[], MATCH(B604,Residents[fullName], 0), 1)</f>
-        <v>2805</v>
+        <v>3073</v>
       </c>
       <c r="D604" t="s">
         <v>9</v>
@@ -12725,7 +12725,7 @@
       </c>
       <c r="C605">
         <f>INDEX(Residents[], MATCH(B605,Residents[fullName], 0), 1)</f>
-        <v>2805</v>
+        <v>3073</v>
       </c>
       <c r="D605" t="s">
         <v>11</v>
@@ -12744,7 +12744,7 @@
       </c>
       <c r="C606">
         <f>INDEX(Residents[], MATCH(B606,Residents[fullName], 0), 1)</f>
-        <v>2805</v>
+        <v>3073</v>
       </c>
       <c r="D606" t="s">
         <v>12</v>
@@ -12763,7 +12763,7 @@
       </c>
       <c r="C607">
         <f>INDEX(Residents[], MATCH(B607,Residents[fullName], 0), 1)</f>
-        <v>2805</v>
+        <v>3073</v>
       </c>
       <c r="D607" t="s">
         <v>13</v>
@@ -12782,7 +12782,7 @@
       </c>
       <c r="C608">
         <f>INDEX(Residents[], MATCH(B608,Residents[fullName], 0), 1)</f>
-        <v>2805</v>
+        <v>3073</v>
       </c>
       <c r="D608" t="s">
         <v>14</v>
@@ -12801,7 +12801,7 @@
       </c>
       <c r="C609">
         <f>INDEX(Residents[], MATCH(B609,Residents[fullName], 0), 1)</f>
-        <v>2805</v>
+        <v>3073</v>
       </c>
       <c r="D609" t="s">
         <v>15</v>
@@ -12820,7 +12820,7 @@
       </c>
       <c r="C610">
         <f>INDEX(Residents[], MATCH(B610,Residents[fullName], 0), 1)</f>
-        <v>2805</v>
+        <v>3073</v>
       </c>
       <c r="D610" t="s">
         <v>16</v>
@@ -12839,7 +12839,7 @@
       </c>
       <c r="C611">
         <f>INDEX(Residents[], MATCH(B611,Residents[fullName], 0), 1)</f>
-        <v>2805</v>
+        <v>3073</v>
       </c>
       <c r="D611" t="s">
         <v>17</v>
@@ -12858,7 +12858,7 @@
       </c>
       <c r="C612">
         <f>INDEX(Residents[], MATCH(B612,Residents[fullName], 0), 1)</f>
-        <v>2805</v>
+        <v>3073</v>
       </c>
       <c r="D612" t="s">
         <v>18</v>
@@ -12877,7 +12877,7 @@
       </c>
       <c r="C613">
         <f>INDEX(Residents[], MATCH(B613,Residents[fullName], 0), 1)</f>
-        <v>2806</v>
+        <v>3074</v>
       </c>
       <c r="D613" t="s">
         <v>4</v>
@@ -12896,7 +12896,7 @@
       </c>
       <c r="C614">
         <f>INDEX(Residents[], MATCH(B614,Residents[fullName], 0), 1)</f>
-        <v>2806</v>
+        <v>3074</v>
       </c>
       <c r="D614" t="s">
         <v>5</v>
@@ -12915,7 +12915,7 @@
       </c>
       <c r="C615">
         <f>INDEX(Residents[], MATCH(B615,Residents[fullName], 0), 1)</f>
-        <v>2806</v>
+        <v>3074</v>
       </c>
       <c r="D615" t="s">
         <v>6</v>
@@ -12934,7 +12934,7 @@
       </c>
       <c r="C616">
         <f>INDEX(Residents[], MATCH(B616,Residents[fullName], 0), 1)</f>
-        <v>2806</v>
+        <v>3074</v>
       </c>
       <c r="D616" t="s">
         <v>7</v>
@@ -12953,7 +12953,7 @@
       </c>
       <c r="C617">
         <f>INDEX(Residents[], MATCH(B617,Residents[fullName], 0), 1)</f>
-        <v>2806</v>
+        <v>3074</v>
       </c>
       <c r="D617" t="s">
         <v>9</v>
@@ -12972,7 +12972,7 @@
       </c>
       <c r="C618">
         <f>INDEX(Residents[], MATCH(B618,Residents[fullName], 0), 1)</f>
-        <v>2806</v>
+        <v>3074</v>
       </c>
       <c r="D618" t="s">
         <v>11</v>
@@ -12991,7 +12991,7 @@
       </c>
       <c r="C619">
         <f>INDEX(Residents[], MATCH(B619,Residents[fullName], 0), 1)</f>
-        <v>2806</v>
+        <v>3074</v>
       </c>
       <c r="D619" t="s">
         <v>12</v>
@@ -13010,7 +13010,7 @@
       </c>
       <c r="C620">
         <f>INDEX(Residents[], MATCH(B620,Residents[fullName], 0), 1)</f>
-        <v>2806</v>
+        <v>3074</v>
       </c>
       <c r="D620" t="s">
         <v>13</v>
@@ -13029,7 +13029,7 @@
       </c>
       <c r="C621">
         <f>INDEX(Residents[], MATCH(B621,Residents[fullName], 0), 1)</f>
-        <v>2806</v>
+        <v>3074</v>
       </c>
       <c r="D621" t="s">
         <v>14</v>
@@ -13048,7 +13048,7 @@
       </c>
       <c r="C622">
         <f>INDEX(Residents[], MATCH(B622,Residents[fullName], 0), 1)</f>
-        <v>2806</v>
+        <v>3074</v>
       </c>
       <c r="D622" t="s">
         <v>15</v>
@@ -13067,7 +13067,7 @@
       </c>
       <c r="C623">
         <f>INDEX(Residents[], MATCH(B623,Residents[fullName], 0), 1)</f>
-        <v>2806</v>
+        <v>3074</v>
       </c>
       <c r="D623" t="s">
         <v>16</v>
@@ -13086,7 +13086,7 @@
       </c>
       <c r="C624">
         <f>INDEX(Residents[], MATCH(B624,Residents[fullName], 0), 1)</f>
-        <v>2806</v>
+        <v>3074</v>
       </c>
       <c r="D624" t="s">
         <v>17</v>
@@ -13105,7 +13105,7 @@
       </c>
       <c r="C625">
         <f>INDEX(Residents[], MATCH(B625,Residents[fullName], 0), 1)</f>
-        <v>2806</v>
+        <v>3074</v>
       </c>
       <c r="D625" t="s">
         <v>18</v>
@@ -13124,7 +13124,7 @@
       </c>
       <c r="C626">
         <f>INDEX(Residents[], MATCH(B626,Residents[fullName], 0), 1)</f>
-        <v>2807</v>
+        <v>3075</v>
       </c>
       <c r="D626" t="s">
         <v>4</v>
@@ -13143,7 +13143,7 @@
       </c>
       <c r="C627">
         <f>INDEX(Residents[], MATCH(B627,Residents[fullName], 0), 1)</f>
-        <v>2807</v>
+        <v>3075</v>
       </c>
       <c r="D627" t="s">
         <v>5</v>
@@ -13162,7 +13162,7 @@
       </c>
       <c r="C628">
         <f>INDEX(Residents[], MATCH(B628,Residents[fullName], 0), 1)</f>
-        <v>2807</v>
+        <v>3075</v>
       </c>
       <c r="D628" t="s">
         <v>6</v>
@@ -13181,7 +13181,7 @@
       </c>
       <c r="C629">
         <f>INDEX(Residents[], MATCH(B629,Residents[fullName], 0), 1)</f>
-        <v>2807</v>
+        <v>3075</v>
       </c>
       <c r="D629" t="s">
         <v>7</v>
@@ -13200,7 +13200,7 @@
       </c>
       <c r="C630">
         <f>INDEX(Residents[], MATCH(B630,Residents[fullName], 0), 1)</f>
-        <v>2807</v>
+        <v>3075</v>
       </c>
       <c r="D630" t="s">
         <v>9</v>
@@ -13219,7 +13219,7 @@
       </c>
       <c r="C631">
         <f>INDEX(Residents[], MATCH(B631,Residents[fullName], 0), 1)</f>
-        <v>2807</v>
+        <v>3075</v>
       </c>
       <c r="D631" t="s">
         <v>11</v>
@@ -13238,7 +13238,7 @@
       </c>
       <c r="C632">
         <f>INDEX(Residents[], MATCH(B632,Residents[fullName], 0), 1)</f>
-        <v>2807</v>
+        <v>3075</v>
       </c>
       <c r="D632" t="s">
         <v>12</v>
@@ -13257,7 +13257,7 @@
       </c>
       <c r="C633">
         <f>INDEX(Residents[], MATCH(B633,Residents[fullName], 0), 1)</f>
-        <v>2807</v>
+        <v>3075</v>
       </c>
       <c r="D633" t="s">
         <v>13</v>
@@ -13276,7 +13276,7 @@
       </c>
       <c r="C634">
         <f>INDEX(Residents[], MATCH(B634,Residents[fullName], 0), 1)</f>
-        <v>2807</v>
+        <v>3075</v>
       </c>
       <c r="D634" t="s">
         <v>14</v>
@@ -13295,7 +13295,7 @@
       </c>
       <c r="C635">
         <f>INDEX(Residents[], MATCH(B635,Residents[fullName], 0), 1)</f>
-        <v>2807</v>
+        <v>3075</v>
       </c>
       <c r="D635" t="s">
         <v>15</v>
@@ -13314,7 +13314,7 @@
       </c>
       <c r="C636">
         <f>INDEX(Residents[], MATCH(B636,Residents[fullName], 0), 1)</f>
-        <v>2807</v>
+        <v>3075</v>
       </c>
       <c r="D636" t="s">
         <v>16</v>
@@ -13333,7 +13333,7 @@
       </c>
       <c r="C637">
         <f>INDEX(Residents[], MATCH(B637,Residents[fullName], 0), 1)</f>
-        <v>2807</v>
+        <v>3075</v>
       </c>
       <c r="D637" t="s">
         <v>17</v>
@@ -13352,7 +13352,7 @@
       </c>
       <c r="C638">
         <f>INDEX(Residents[], MATCH(B638,Residents[fullName], 0), 1)</f>
-        <v>2807</v>
+        <v>3075</v>
       </c>
       <c r="D638" t="s">
         <v>18</v>
@@ -13371,7 +13371,7 @@
       </c>
       <c r="C639">
         <f>INDEX(Residents[], MATCH(B639,Residents[fullName], 0), 1)</f>
-        <v>2808</v>
+        <v>3076</v>
       </c>
       <c r="D639" t="s">
         <v>4</v>
@@ -13390,7 +13390,7 @@
       </c>
       <c r="C640">
         <f>INDEX(Residents[], MATCH(B640,Residents[fullName], 0), 1)</f>
-        <v>2808</v>
+        <v>3076</v>
       </c>
       <c r="D640" t="s">
         <v>5</v>
@@ -13409,7 +13409,7 @@
       </c>
       <c r="C641">
         <f>INDEX(Residents[], MATCH(B641,Residents[fullName], 0), 1)</f>
-        <v>2808</v>
+        <v>3076</v>
       </c>
       <c r="D641" t="s">
         <v>6</v>
@@ -13428,7 +13428,7 @@
       </c>
       <c r="C642">
         <f>INDEX(Residents[], MATCH(B642,Residents[fullName], 0), 1)</f>
-        <v>2808</v>
+        <v>3076</v>
       </c>
       <c r="D642" t="s">
         <v>7</v>
@@ -13447,7 +13447,7 @@
       </c>
       <c r="C643">
         <f>INDEX(Residents[], MATCH(B643,Residents[fullName], 0), 1)</f>
-        <v>2808</v>
+        <v>3076</v>
       </c>
       <c r="D643" t="s">
         <v>9</v>
@@ -13466,7 +13466,7 @@
       </c>
       <c r="C644">
         <f>INDEX(Residents[], MATCH(B644,Residents[fullName], 0), 1)</f>
-        <v>2808</v>
+        <v>3076</v>
       </c>
       <c r="D644" t="s">
         <v>11</v>
@@ -13485,7 +13485,7 @@
       </c>
       <c r="C645">
         <f>INDEX(Residents[], MATCH(B645,Residents[fullName], 0), 1)</f>
-        <v>2808</v>
+        <v>3076</v>
       </c>
       <c r="D645" t="s">
         <v>12</v>
@@ -13504,7 +13504,7 @@
       </c>
       <c r="C646">
         <f>INDEX(Residents[], MATCH(B646,Residents[fullName], 0), 1)</f>
-        <v>2808</v>
+        <v>3076</v>
       </c>
       <c r="D646" t="s">
         <v>13</v>
@@ -13523,7 +13523,7 @@
       </c>
       <c r="C647">
         <f>INDEX(Residents[], MATCH(B647,Residents[fullName], 0), 1)</f>
-        <v>2808</v>
+        <v>3076</v>
       </c>
       <c r="D647" t="s">
         <v>14</v>
@@ -13542,7 +13542,7 @@
       </c>
       <c r="C648">
         <f>INDEX(Residents[], MATCH(B648,Residents[fullName], 0), 1)</f>
-        <v>2808</v>
+        <v>3076</v>
       </c>
       <c r="D648" t="s">
         <v>15</v>
@@ -13561,7 +13561,7 @@
       </c>
       <c r="C649">
         <f>INDEX(Residents[], MATCH(B649,Residents[fullName], 0), 1)</f>
-        <v>2808</v>
+        <v>3076</v>
       </c>
       <c r="D649" t="s">
         <v>16</v>
@@ -13580,7 +13580,7 @@
       </c>
       <c r="C650">
         <f>INDEX(Residents[], MATCH(B650,Residents[fullName], 0), 1)</f>
-        <v>2808</v>
+        <v>3076</v>
       </c>
       <c r="D650" t="s">
         <v>17</v>
@@ -13599,7 +13599,7 @@
       </c>
       <c r="C651">
         <f>INDEX(Residents[], MATCH(B651,Residents[fullName], 0), 1)</f>
-        <v>2808</v>
+        <v>3076</v>
       </c>
       <c r="D651" t="s">
         <v>18</v>
@@ -13618,7 +13618,7 @@
       </c>
       <c r="C652">
         <f>INDEX(Residents[], MATCH(B652,Residents[fullName], 0), 1)</f>
-        <v>2809</v>
+        <v>3077</v>
       </c>
       <c r="D652" t="s">
         <v>4</v>
@@ -13637,7 +13637,7 @@
       </c>
       <c r="C653">
         <f>INDEX(Residents[], MATCH(B653,Residents[fullName], 0), 1)</f>
-        <v>2809</v>
+        <v>3077</v>
       </c>
       <c r="D653" t="s">
         <v>5</v>
@@ -13656,7 +13656,7 @@
       </c>
       <c r="C654">
         <f>INDEX(Residents[], MATCH(B654,Residents[fullName], 0), 1)</f>
-        <v>2809</v>
+        <v>3077</v>
       </c>
       <c r="D654" t="s">
         <v>6</v>
@@ -13675,7 +13675,7 @@
       </c>
       <c r="C655">
         <f>INDEX(Residents[], MATCH(B655,Residents[fullName], 0), 1)</f>
-        <v>2809</v>
+        <v>3077</v>
       </c>
       <c r="D655" t="s">
         <v>7</v>
@@ -13694,7 +13694,7 @@
       </c>
       <c r="C656">
         <f>INDEX(Residents[], MATCH(B656,Residents[fullName], 0), 1)</f>
-        <v>2809</v>
+        <v>3077</v>
       </c>
       <c r="D656" t="s">
         <v>9</v>
@@ -13713,7 +13713,7 @@
       </c>
       <c r="C657">
         <f>INDEX(Residents[], MATCH(B657,Residents[fullName], 0), 1)</f>
-        <v>2809</v>
+        <v>3077</v>
       </c>
       <c r="D657" t="s">
         <v>11</v>
@@ -13732,7 +13732,7 @@
       </c>
       <c r="C658">
         <f>INDEX(Residents[], MATCH(B658,Residents[fullName], 0), 1)</f>
-        <v>2809</v>
+        <v>3077</v>
       </c>
       <c r="D658" t="s">
         <v>12</v>
@@ -13751,7 +13751,7 @@
       </c>
       <c r="C659">
         <f>INDEX(Residents[], MATCH(B659,Residents[fullName], 0), 1)</f>
-        <v>2809</v>
+        <v>3077</v>
       </c>
       <c r="D659" t="s">
         <v>13</v>
@@ -13770,7 +13770,7 @@
       </c>
       <c r="C660">
         <f>INDEX(Residents[], MATCH(B660,Residents[fullName], 0), 1)</f>
-        <v>2809</v>
+        <v>3077</v>
       </c>
       <c r="D660" t="s">
         <v>14</v>
@@ -13789,7 +13789,7 @@
       </c>
       <c r="C661">
         <f>INDEX(Residents[], MATCH(B661,Residents[fullName], 0), 1)</f>
-        <v>2809</v>
+        <v>3077</v>
       </c>
       <c r="D661" t="s">
         <v>15</v>
@@ -13808,7 +13808,7 @@
       </c>
       <c r="C662">
         <f>INDEX(Residents[], MATCH(B662,Residents[fullName], 0), 1)</f>
-        <v>2809</v>
+        <v>3077</v>
       </c>
       <c r="D662" t="s">
         <v>16</v>
@@ -13827,7 +13827,7 @@
       </c>
       <c r="C663">
         <f>INDEX(Residents[], MATCH(B663,Residents[fullName], 0), 1)</f>
-        <v>2809</v>
+        <v>3077</v>
       </c>
       <c r="D663" t="s">
         <v>17</v>
@@ -13846,7 +13846,7 @@
       </c>
       <c r="C664">
         <f>INDEX(Residents[], MATCH(B664,Residents[fullName], 0), 1)</f>
-        <v>2809</v>
+        <v>3077</v>
       </c>
       <c r="D664" t="s">
         <v>18</v>
@@ -13865,7 +13865,7 @@
       </c>
       <c r="C665">
         <f>INDEX(Residents[], MATCH(B665,Residents[fullName], 0), 1)</f>
-        <v>2810</v>
+        <v>3078</v>
       </c>
       <c r="D665" t="s">
         <v>4</v>
@@ -13884,7 +13884,7 @@
       </c>
       <c r="C666">
         <f>INDEX(Residents[], MATCH(B666,Residents[fullName], 0), 1)</f>
-        <v>2810</v>
+        <v>3078</v>
       </c>
       <c r="D666" t="s">
         <v>5</v>
@@ -13903,7 +13903,7 @@
       </c>
       <c r="C667">
         <f>INDEX(Residents[], MATCH(B667,Residents[fullName], 0), 1)</f>
-        <v>2810</v>
+        <v>3078</v>
       </c>
       <c r="D667" t="s">
         <v>6</v>
@@ -13922,7 +13922,7 @@
       </c>
       <c r="C668">
         <f>INDEX(Residents[], MATCH(B668,Residents[fullName], 0), 1)</f>
-        <v>2810</v>
+        <v>3078</v>
       </c>
       <c r="D668" t="s">
         <v>7</v>
@@ -13941,7 +13941,7 @@
       </c>
       <c r="C669">
         <f>INDEX(Residents[], MATCH(B669,Residents[fullName], 0), 1)</f>
-        <v>2810</v>
+        <v>3078</v>
       </c>
       <c r="D669" t="s">
         <v>9</v>
@@ -13960,7 +13960,7 @@
       </c>
       <c r="C670">
         <f>INDEX(Residents[], MATCH(B670,Residents[fullName], 0), 1)</f>
-        <v>2810</v>
+        <v>3078</v>
       </c>
       <c r="D670" t="s">
         <v>11</v>
@@ -13979,7 +13979,7 @@
       </c>
       <c r="C671">
         <f>INDEX(Residents[], MATCH(B671,Residents[fullName], 0), 1)</f>
-        <v>2810</v>
+        <v>3078</v>
       </c>
       <c r="D671" t="s">
         <v>12</v>
@@ -13998,7 +13998,7 @@
       </c>
       <c r="C672">
         <f>INDEX(Residents[], MATCH(B672,Residents[fullName], 0), 1)</f>
-        <v>2810</v>
+        <v>3078</v>
       </c>
       <c r="D672" t="s">
         <v>13</v>
@@ -14017,7 +14017,7 @@
       </c>
       <c r="C673">
         <f>INDEX(Residents[], MATCH(B673,Residents[fullName], 0), 1)</f>
-        <v>2810</v>
+        <v>3078</v>
       </c>
       <c r="D673" t="s">
         <v>14</v>
@@ -14036,7 +14036,7 @@
       </c>
       <c r="C674">
         <f>INDEX(Residents[], MATCH(B674,Residents[fullName], 0), 1)</f>
-        <v>2810</v>
+        <v>3078</v>
       </c>
       <c r="D674" t="s">
         <v>15</v>
@@ -14055,7 +14055,7 @@
       </c>
       <c r="C675">
         <f>INDEX(Residents[], MATCH(B675,Residents[fullName], 0), 1)</f>
-        <v>2810</v>
+        <v>3078</v>
       </c>
       <c r="D675" t="s">
         <v>16</v>
@@ -14074,7 +14074,7 @@
       </c>
       <c r="C676">
         <f>INDEX(Residents[], MATCH(B676,Residents[fullName], 0), 1)</f>
-        <v>2810</v>
+        <v>3078</v>
       </c>
       <c r="D676" t="s">
         <v>17</v>
@@ -14093,7 +14093,7 @@
       </c>
       <c r="C677">
         <f>INDEX(Residents[], MATCH(B677,Residents[fullName], 0), 1)</f>
-        <v>2810</v>
+        <v>3078</v>
       </c>
       <c r="D677" t="s">
         <v>18</v>
@@ -14112,7 +14112,7 @@
       </c>
       <c r="C678">
         <f>INDEX(Residents[], MATCH(B678,Residents[fullName], 0), 1)</f>
-        <v>2811</v>
+        <v>3079</v>
       </c>
       <c r="D678" t="s">
         <v>4</v>
@@ -14131,7 +14131,7 @@
       </c>
       <c r="C679">
         <f>INDEX(Residents[], MATCH(B679,Residents[fullName], 0), 1)</f>
-        <v>2811</v>
+        <v>3079</v>
       </c>
       <c r="D679" t="s">
         <v>5</v>
@@ -14150,7 +14150,7 @@
       </c>
       <c r="C680">
         <f>INDEX(Residents[], MATCH(B680,Residents[fullName], 0), 1)</f>
-        <v>2811</v>
+        <v>3079</v>
       </c>
       <c r="D680" t="s">
         <v>6</v>
@@ -14169,7 +14169,7 @@
       </c>
       <c r="C681">
         <f>INDEX(Residents[], MATCH(B681,Residents[fullName], 0), 1)</f>
-        <v>2811</v>
+        <v>3079</v>
       </c>
       <c r="D681" t="s">
         <v>7</v>
@@ -14188,7 +14188,7 @@
       </c>
       <c r="C682">
         <f>INDEX(Residents[], MATCH(B682,Residents[fullName], 0), 1)</f>
-        <v>2811</v>
+        <v>3079</v>
       </c>
       <c r="D682" t="s">
         <v>9</v>
@@ -14207,7 +14207,7 @@
       </c>
       <c r="C683">
         <f>INDEX(Residents[], MATCH(B683,Residents[fullName], 0), 1)</f>
-        <v>2811</v>
+        <v>3079</v>
       </c>
       <c r="D683" t="s">
         <v>11</v>
@@ -14226,7 +14226,7 @@
       </c>
       <c r="C684">
         <f>INDEX(Residents[], MATCH(B684,Residents[fullName], 0), 1)</f>
-        <v>2811</v>
+        <v>3079</v>
       </c>
       <c r="D684" t="s">
         <v>12</v>
@@ -14245,7 +14245,7 @@
       </c>
       <c r="C685">
         <f>INDEX(Residents[], MATCH(B685,Residents[fullName], 0), 1)</f>
-        <v>2811</v>
+        <v>3079</v>
       </c>
       <c r="D685" t="s">
         <v>13</v>
@@ -14264,7 +14264,7 @@
       </c>
       <c r="C686">
         <f>INDEX(Residents[], MATCH(B686,Residents[fullName], 0), 1)</f>
-        <v>2811</v>
+        <v>3079</v>
       </c>
       <c r="D686" t="s">
         <v>14</v>
@@ -14283,7 +14283,7 @@
       </c>
       <c r="C687">
         <f>INDEX(Residents[], MATCH(B687,Residents[fullName], 0), 1)</f>
-        <v>2811</v>
+        <v>3079</v>
       </c>
       <c r="D687" t="s">
         <v>15</v>
@@ -14302,7 +14302,7 @@
       </c>
       <c r="C688">
         <f>INDEX(Residents[], MATCH(B688,Residents[fullName], 0), 1)</f>
-        <v>2811</v>
+        <v>3079</v>
       </c>
       <c r="D688" t="s">
         <v>16</v>
@@ -14321,7 +14321,7 @@
       </c>
       <c r="C689">
         <f>INDEX(Residents[], MATCH(B689,Residents[fullName], 0), 1)</f>
-        <v>2811</v>
+        <v>3079</v>
       </c>
       <c r="D689" t="s">
         <v>17</v>
@@ -14340,7 +14340,7 @@
       </c>
       <c r="C690">
         <f>INDEX(Residents[], MATCH(B690,Residents[fullName], 0), 1)</f>
-        <v>2811</v>
+        <v>3079</v>
       </c>
       <c r="D690" t="s">
         <v>18</v>
@@ -14359,7 +14359,7 @@
       </c>
       <c r="C691">
         <f>INDEX(Residents[], MATCH(B691,Residents[fullName], 0), 1)</f>
-        <v>2812</v>
+        <v>3080</v>
       </c>
       <c r="D691" t="s">
         <v>4</v>
@@ -14378,7 +14378,7 @@
       </c>
       <c r="C692">
         <f>INDEX(Residents[], MATCH(B692,Residents[fullName], 0), 1)</f>
-        <v>2812</v>
+        <v>3080</v>
       </c>
       <c r="D692" t="s">
         <v>5</v>
@@ -14397,7 +14397,7 @@
       </c>
       <c r="C693">
         <f>INDEX(Residents[], MATCH(B693,Residents[fullName], 0), 1)</f>
-        <v>2812</v>
+        <v>3080</v>
       </c>
       <c r="D693" t="s">
         <v>6</v>
@@ -14416,7 +14416,7 @@
       </c>
       <c r="C694">
         <f>INDEX(Residents[], MATCH(B694,Residents[fullName], 0), 1)</f>
-        <v>2812</v>
+        <v>3080</v>
       </c>
       <c r="D694" t="s">
         <v>7</v>
@@ -14435,7 +14435,7 @@
       </c>
       <c r="C695">
         <f>INDEX(Residents[], MATCH(B695,Residents[fullName], 0), 1)</f>
-        <v>2812</v>
+        <v>3080</v>
       </c>
       <c r="D695" t="s">
         <v>9</v>
@@ -14454,7 +14454,7 @@
       </c>
       <c r="C696">
         <f>INDEX(Residents[], MATCH(B696,Residents[fullName], 0), 1)</f>
-        <v>2812</v>
+        <v>3080</v>
       </c>
       <c r="D696" t="s">
         <v>11</v>
@@ -14473,7 +14473,7 @@
       </c>
       <c r="C697">
         <f>INDEX(Residents[], MATCH(B697,Residents[fullName], 0), 1)</f>
-        <v>2812</v>
+        <v>3080</v>
       </c>
       <c r="D697" t="s">
         <v>12</v>
@@ -14492,7 +14492,7 @@
       </c>
       <c r="C698">
         <f>INDEX(Residents[], MATCH(B698,Residents[fullName], 0), 1)</f>
-        <v>2812</v>
+        <v>3080</v>
       </c>
       <c r="D698" t="s">
         <v>13</v>
@@ -14511,7 +14511,7 @@
       </c>
       <c r="C699">
         <f>INDEX(Residents[], MATCH(B699,Residents[fullName], 0), 1)</f>
-        <v>2812</v>
+        <v>3080</v>
       </c>
       <c r="D699" t="s">
         <v>14</v>
@@ -14530,7 +14530,7 @@
       </c>
       <c r="C700">
         <f>INDEX(Residents[], MATCH(B700,Residents[fullName], 0), 1)</f>
-        <v>2812</v>
+        <v>3080</v>
       </c>
       <c r="D700" t="s">
         <v>15</v>
@@ -14549,7 +14549,7 @@
       </c>
       <c r="C701">
         <f>INDEX(Residents[], MATCH(B701,Residents[fullName], 0), 1)</f>
-        <v>2812</v>
+        <v>3080</v>
       </c>
       <c r="D701" t="s">
         <v>16</v>
@@ -14568,7 +14568,7 @@
       </c>
       <c r="C702">
         <f>INDEX(Residents[], MATCH(B702,Residents[fullName], 0), 1)</f>
-        <v>2812</v>
+        <v>3080</v>
       </c>
       <c r="D702" t="s">
         <v>17</v>
@@ -14587,7 +14587,7 @@
       </c>
       <c r="C703">
         <f>INDEX(Residents[], MATCH(B703,Residents[fullName], 0), 1)</f>
-        <v>2812</v>
+        <v>3080</v>
       </c>
       <c r="D703" t="s">
         <v>18</v>
@@ -14606,7 +14606,7 @@
       </c>
       <c r="C704">
         <f>INDEX(Residents[], MATCH(B704,Residents[fullName], 0), 1)</f>
-        <v>2813</v>
+        <v>3081</v>
       </c>
       <c r="D704" t="s">
         <v>4</v>
@@ -14625,7 +14625,7 @@
       </c>
       <c r="C705">
         <f>INDEX(Residents[], MATCH(B705,Residents[fullName], 0), 1)</f>
-        <v>2813</v>
+        <v>3081</v>
       </c>
       <c r="D705" t="s">
         <v>5</v>
@@ -14644,7 +14644,7 @@
       </c>
       <c r="C706">
         <f>INDEX(Residents[], MATCH(B706,Residents[fullName], 0), 1)</f>
-        <v>2813</v>
+        <v>3081</v>
       </c>
       <c r="D706" t="s">
         <v>6</v>
@@ -14663,7 +14663,7 @@
       </c>
       <c r="C707">
         <f>INDEX(Residents[], MATCH(B707,Residents[fullName], 0), 1)</f>
-        <v>2813</v>
+        <v>3081</v>
       </c>
       <c r="D707" t="s">
         <v>7</v>
@@ -14682,7 +14682,7 @@
       </c>
       <c r="C708">
         <f>INDEX(Residents[], MATCH(B708,Residents[fullName], 0), 1)</f>
-        <v>2813</v>
+        <v>3081</v>
       </c>
       <c r="D708" t="s">
         <v>9</v>
@@ -14701,7 +14701,7 @@
       </c>
       <c r="C709">
         <f>INDEX(Residents[], MATCH(B709,Residents[fullName], 0), 1)</f>
-        <v>2813</v>
+        <v>3081</v>
       </c>
       <c r="D709" t="s">
         <v>11</v>
@@ -14720,7 +14720,7 @@
       </c>
       <c r="C710">
         <f>INDEX(Residents[], MATCH(B710,Residents[fullName], 0), 1)</f>
-        <v>2813</v>
+        <v>3081</v>
       </c>
       <c r="D710" t="s">
         <v>12</v>
@@ -14739,7 +14739,7 @@
       </c>
       <c r="C711">
         <f>INDEX(Residents[], MATCH(B711,Residents[fullName], 0), 1)</f>
-        <v>2813</v>
+        <v>3081</v>
       </c>
       <c r="D711" t="s">
         <v>13</v>
@@ -14758,7 +14758,7 @@
       </c>
       <c r="C712">
         <f>INDEX(Residents[], MATCH(B712,Residents[fullName], 0), 1)</f>
-        <v>2813</v>
+        <v>3081</v>
       </c>
       <c r="D712" t="s">
         <v>14</v>
@@ -14777,7 +14777,7 @@
       </c>
       <c r="C713">
         <f>INDEX(Residents[], MATCH(B713,Residents[fullName], 0), 1)</f>
-        <v>2813</v>
+        <v>3081</v>
       </c>
       <c r="D713" t="s">
         <v>15</v>
@@ -14796,7 +14796,7 @@
       </c>
       <c r="C714">
         <f>INDEX(Residents[], MATCH(B714,Residents[fullName], 0), 1)</f>
-        <v>2813</v>
+        <v>3081</v>
       </c>
       <c r="D714" t="s">
         <v>16</v>
@@ -14815,7 +14815,7 @@
       </c>
       <c r="C715">
         <f>INDEX(Residents[], MATCH(B715,Residents[fullName], 0), 1)</f>
-        <v>2813</v>
+        <v>3081</v>
       </c>
       <c r="D715" t="s">
         <v>17</v>
@@ -14834,7 +14834,7 @@
       </c>
       <c r="C716">
         <f>INDEX(Residents[], MATCH(B716,Residents[fullName], 0), 1)</f>
-        <v>2813</v>
+        <v>3081</v>
       </c>
       <c r="D716" t="s">
         <v>18</v>
@@ -14853,7 +14853,7 @@
       </c>
       <c r="C717">
         <f>INDEX(Residents[], MATCH(B717,Residents[fullName], 0), 1)</f>
-        <v>2814</v>
+        <v>3082</v>
       </c>
       <c r="D717" t="s">
         <v>4</v>
@@ -14872,7 +14872,7 @@
       </c>
       <c r="C718">
         <f>INDEX(Residents[], MATCH(B718,Residents[fullName], 0), 1)</f>
-        <v>2814</v>
+        <v>3082</v>
       </c>
       <c r="D718" t="s">
         <v>5</v>
@@ -14891,7 +14891,7 @@
       </c>
       <c r="C719">
         <f>INDEX(Residents[], MATCH(B719,Residents[fullName], 0), 1)</f>
-        <v>2814</v>
+        <v>3082</v>
       </c>
       <c r="D719" t="s">
         <v>6</v>
@@ -14910,7 +14910,7 @@
       </c>
       <c r="C720">
         <f>INDEX(Residents[], MATCH(B720,Residents[fullName], 0), 1)</f>
-        <v>2814</v>
+        <v>3082</v>
       </c>
       <c r="D720" t="s">
         <v>7</v>
@@ -14929,7 +14929,7 @@
       </c>
       <c r="C721">
         <f>INDEX(Residents[], MATCH(B721,Residents[fullName], 0), 1)</f>
-        <v>2814</v>
+        <v>3082</v>
       </c>
       <c r="D721" t="s">
         <v>9</v>
@@ -14948,7 +14948,7 @@
       </c>
       <c r="C722">
         <f>INDEX(Residents[], MATCH(B722,Residents[fullName], 0), 1)</f>
-        <v>2814</v>
+        <v>3082</v>
       </c>
       <c r="D722" t="s">
         <v>11</v>
@@ -14967,7 +14967,7 @@
       </c>
       <c r="C723">
         <f>INDEX(Residents[], MATCH(B723,Residents[fullName], 0), 1)</f>
-        <v>2814</v>
+        <v>3082</v>
       </c>
       <c r="D723" t="s">
         <v>12</v>
@@ -14986,7 +14986,7 @@
       </c>
       <c r="C724">
         <f>INDEX(Residents[], MATCH(B724,Residents[fullName], 0), 1)</f>
-        <v>2814</v>
+        <v>3082</v>
       </c>
       <c r="D724" t="s">
         <v>13</v>
@@ -15005,7 +15005,7 @@
       </c>
       <c r="C725">
         <f>INDEX(Residents[], MATCH(B725,Residents[fullName], 0), 1)</f>
-        <v>2814</v>
+        <v>3082</v>
       </c>
       <c r="D725" t="s">
         <v>14</v>
@@ -15024,7 +15024,7 @@
       </c>
       <c r="C726">
         <f>INDEX(Residents[], MATCH(B726,Residents[fullName], 0), 1)</f>
-        <v>2814</v>
+        <v>3082</v>
       </c>
       <c r="D726" t="s">
         <v>15</v>
@@ -15043,7 +15043,7 @@
       </c>
       <c r="C727">
         <f>INDEX(Residents[], MATCH(B727,Residents[fullName], 0), 1)</f>
-        <v>2814</v>
+        <v>3082</v>
       </c>
       <c r="D727" t="s">
         <v>16</v>
@@ -15062,7 +15062,7 @@
       </c>
       <c r="C728">
         <f>INDEX(Residents[], MATCH(B728,Residents[fullName], 0), 1)</f>
-        <v>2814</v>
+        <v>3082</v>
       </c>
       <c r="D728" t="s">
         <v>17</v>
@@ -15081,7 +15081,7 @@
       </c>
       <c r="C729">
         <f>INDEX(Residents[], MATCH(B729,Residents[fullName], 0), 1)</f>
-        <v>2814</v>
+        <v>3082</v>
       </c>
       <c r="D729" t="s">
         <v>18</v>
@@ -15100,7 +15100,7 @@
       </c>
       <c r="C730">
         <f>INDEX(Residents[], MATCH(B730,Residents[fullName], 0), 1)</f>
-        <v>2815</v>
+        <v>3083</v>
       </c>
       <c r="D730" t="s">
         <v>4</v>
@@ -15119,7 +15119,7 @@
       </c>
       <c r="C731">
         <f>INDEX(Residents[], MATCH(B731,Residents[fullName], 0), 1)</f>
-        <v>2815</v>
+        <v>3083</v>
       </c>
       <c r="D731" t="s">
         <v>5</v>
@@ -15138,7 +15138,7 @@
       </c>
       <c r="C732">
         <f>INDEX(Residents[], MATCH(B732,Residents[fullName], 0), 1)</f>
-        <v>2815</v>
+        <v>3083</v>
       </c>
       <c r="D732" t="s">
         <v>6</v>
@@ -15157,7 +15157,7 @@
       </c>
       <c r="C733">
         <f>INDEX(Residents[], MATCH(B733,Residents[fullName], 0), 1)</f>
-        <v>2815</v>
+        <v>3083</v>
       </c>
       <c r="D733" t="s">
         <v>7</v>
@@ -15176,7 +15176,7 @@
       </c>
       <c r="C734">
         <f>INDEX(Residents[], MATCH(B734,Residents[fullName], 0), 1)</f>
-        <v>2815</v>
+        <v>3083</v>
       </c>
       <c r="D734" t="s">
         <v>9</v>
@@ -15195,7 +15195,7 @@
       </c>
       <c r="C735">
         <f>INDEX(Residents[], MATCH(B735,Residents[fullName], 0), 1)</f>
-        <v>2815</v>
+        <v>3083</v>
       </c>
       <c r="D735" t="s">
         <v>11</v>
@@ -15214,7 +15214,7 @@
       </c>
       <c r="C736">
         <f>INDEX(Residents[], MATCH(B736,Residents[fullName], 0), 1)</f>
-        <v>2815</v>
+        <v>3083</v>
       </c>
       <c r="D736" t="s">
         <v>12</v>
@@ -15233,7 +15233,7 @@
       </c>
       <c r="C737">
         <f>INDEX(Residents[], MATCH(B737,Residents[fullName], 0), 1)</f>
-        <v>2815</v>
+        <v>3083</v>
       </c>
       <c r="D737" t="s">
         <v>13</v>
@@ -15252,7 +15252,7 @@
       </c>
       <c r="C738">
         <f>INDEX(Residents[], MATCH(B738,Residents[fullName], 0), 1)</f>
-        <v>2815</v>
+        <v>3083</v>
       </c>
       <c r="D738" t="s">
         <v>14</v>
@@ -15271,7 +15271,7 @@
       </c>
       <c r="C739">
         <f>INDEX(Residents[], MATCH(B739,Residents[fullName], 0), 1)</f>
-        <v>2815</v>
+        <v>3083</v>
       </c>
       <c r="D739" t="s">
         <v>15</v>
@@ -15290,7 +15290,7 @@
       </c>
       <c r="C740">
         <f>INDEX(Residents[], MATCH(B740,Residents[fullName], 0), 1)</f>
-        <v>2815</v>
+        <v>3083</v>
       </c>
       <c r="D740" t="s">
         <v>16</v>
@@ -15309,7 +15309,7 @@
       </c>
       <c r="C741">
         <f>INDEX(Residents[], MATCH(B741,Residents[fullName], 0), 1)</f>
-        <v>2815</v>
+        <v>3083</v>
       </c>
       <c r="D741" t="s">
         <v>17</v>
@@ -15328,7 +15328,7 @@
       </c>
       <c r="C742">
         <f>INDEX(Residents[], MATCH(B742,Residents[fullName], 0), 1)</f>
-        <v>2815</v>
+        <v>3083</v>
       </c>
       <c r="D742" t="s">
         <v>18</v>
@@ -15347,7 +15347,7 @@
       </c>
       <c r="C743">
         <f>INDEX(Residents[], MATCH(B743,Residents[fullName], 0), 1)</f>
-        <v>2816</v>
+        <v>3084</v>
       </c>
       <c r="D743" t="s">
         <v>4</v>
@@ -15366,7 +15366,7 @@
       </c>
       <c r="C744">
         <f>INDEX(Residents[], MATCH(B744,Residents[fullName], 0), 1)</f>
-        <v>2816</v>
+        <v>3084</v>
       </c>
       <c r="D744" t="s">
         <v>5</v>
@@ -15385,7 +15385,7 @@
       </c>
       <c r="C745">
         <f>INDEX(Residents[], MATCH(B745,Residents[fullName], 0), 1)</f>
-        <v>2816</v>
+        <v>3084</v>
       </c>
       <c r="D745" t="s">
         <v>6</v>
@@ -15404,7 +15404,7 @@
       </c>
       <c r="C746">
         <f>INDEX(Residents[], MATCH(B746,Residents[fullName], 0), 1)</f>
-        <v>2816</v>
+        <v>3084</v>
       </c>
       <c r="D746" t="s">
         <v>7</v>
@@ -15423,7 +15423,7 @@
       </c>
       <c r="C747">
         <f>INDEX(Residents[], MATCH(B747,Residents[fullName], 0), 1)</f>
-        <v>2816</v>
+        <v>3084</v>
       </c>
       <c r="D747" t="s">
         <v>9</v>
@@ -15442,7 +15442,7 @@
       </c>
       <c r="C748">
         <f>INDEX(Residents[], MATCH(B748,Residents[fullName], 0), 1)</f>
-        <v>2816</v>
+        <v>3084</v>
       </c>
       <c r="D748" t="s">
         <v>11</v>
@@ -15461,7 +15461,7 @@
       </c>
       <c r="C749">
         <f>INDEX(Residents[], MATCH(B749,Residents[fullName], 0), 1)</f>
-        <v>2816</v>
+        <v>3084</v>
       </c>
       <c r="D749" t="s">
         <v>12</v>
@@ -15480,7 +15480,7 @@
       </c>
       <c r="C750">
         <f>INDEX(Residents[], MATCH(B750,Residents[fullName], 0), 1)</f>
-        <v>2816</v>
+        <v>3084</v>
       </c>
       <c r="D750" t="s">
         <v>13</v>
@@ -15499,7 +15499,7 @@
       </c>
       <c r="C751">
         <f>INDEX(Residents[], MATCH(B751,Residents[fullName], 0), 1)</f>
-        <v>2816</v>
+        <v>3084</v>
       </c>
       <c r="D751" t="s">
         <v>14</v>
@@ -15518,7 +15518,7 @@
       </c>
       <c r="C752">
         <f>INDEX(Residents[], MATCH(B752,Residents[fullName], 0), 1)</f>
-        <v>2816</v>
+        <v>3084</v>
       </c>
       <c r="D752" t="s">
         <v>15</v>
@@ -15537,7 +15537,7 @@
       </c>
       <c r="C753">
         <f>INDEX(Residents[], MATCH(B753,Residents[fullName], 0), 1)</f>
-        <v>2816</v>
+        <v>3084</v>
       </c>
       <c r="D753" t="s">
         <v>16</v>
@@ -15556,7 +15556,7 @@
       </c>
       <c r="C754">
         <f>INDEX(Residents[], MATCH(B754,Residents[fullName], 0), 1)</f>
-        <v>2816</v>
+        <v>3084</v>
       </c>
       <c r="D754" t="s">
         <v>17</v>
@@ -15575,7 +15575,7 @@
       </c>
       <c r="C755">
         <f>INDEX(Residents[], MATCH(B755,Residents[fullName], 0), 1)</f>
-        <v>2816</v>
+        <v>3084</v>
       </c>
       <c r="D755" t="s">
         <v>18</v>
@@ -15594,7 +15594,7 @@
       </c>
       <c r="C756">
         <f>INDEX(Residents[], MATCH(B756,Residents[fullName], 0), 1)</f>
-        <v>2817</v>
+        <v>3085</v>
       </c>
       <c r="D756" t="s">
         <v>4</v>
@@ -15613,7 +15613,7 @@
       </c>
       <c r="C757">
         <f>INDEX(Residents[], MATCH(B757,Residents[fullName], 0), 1)</f>
-        <v>2817</v>
+        <v>3085</v>
       </c>
       <c r="D757" t="s">
         <v>5</v>
@@ -15632,7 +15632,7 @@
       </c>
       <c r="C758">
         <f>INDEX(Residents[], MATCH(B758,Residents[fullName], 0), 1)</f>
-        <v>2817</v>
+        <v>3085</v>
       </c>
       <c r="D758" t="s">
         <v>6</v>
@@ -15651,7 +15651,7 @@
       </c>
       <c r="C759">
         <f>INDEX(Residents[], MATCH(B759,Residents[fullName], 0), 1)</f>
-        <v>2817</v>
+        <v>3085</v>
       </c>
       <c r="D759" t="s">
         <v>7</v>
@@ -15670,7 +15670,7 @@
       </c>
       <c r="C760">
         <f>INDEX(Residents[], MATCH(B760,Residents[fullName], 0), 1)</f>
-        <v>2817</v>
+        <v>3085</v>
       </c>
       <c r="D760" t="s">
         <v>9</v>
@@ -15689,7 +15689,7 @@
       </c>
       <c r="C761">
         <f>INDEX(Residents[], MATCH(B761,Residents[fullName], 0), 1)</f>
-        <v>2817</v>
+        <v>3085</v>
       </c>
       <c r="D761" t="s">
         <v>11</v>
@@ -15708,7 +15708,7 @@
       </c>
       <c r="C762">
         <f>INDEX(Residents[], MATCH(B762,Residents[fullName], 0), 1)</f>
-        <v>2817</v>
+        <v>3085</v>
       </c>
       <c r="D762" t="s">
         <v>12</v>
@@ -15727,7 +15727,7 @@
       </c>
       <c r="C763">
         <f>INDEX(Residents[], MATCH(B763,Residents[fullName], 0), 1)</f>
-        <v>2817</v>
+        <v>3085</v>
       </c>
       <c r="D763" t="s">
         <v>13</v>
@@ -15746,7 +15746,7 @@
       </c>
       <c r="C764">
         <f>INDEX(Residents[], MATCH(B764,Residents[fullName], 0), 1)</f>
-        <v>2817</v>
+        <v>3085</v>
       </c>
       <c r="D764" t="s">
         <v>14</v>
@@ -15765,7 +15765,7 @@
       </c>
       <c r="C765">
         <f>INDEX(Residents[], MATCH(B765,Residents[fullName], 0), 1)</f>
-        <v>2817</v>
+        <v>3085</v>
       </c>
       <c r="D765" t="s">
         <v>15</v>
@@ -15784,7 +15784,7 @@
       </c>
       <c r="C766">
         <f>INDEX(Residents[], MATCH(B766,Residents[fullName], 0), 1)</f>
-        <v>2817</v>
+        <v>3085</v>
       </c>
       <c r="D766" t="s">
         <v>16</v>
@@ -15803,7 +15803,7 @@
       </c>
       <c r="C767">
         <f>INDEX(Residents[], MATCH(B767,Residents[fullName], 0), 1)</f>
-        <v>2817</v>
+        <v>3085</v>
       </c>
       <c r="D767" t="s">
         <v>17</v>
@@ -15822,7 +15822,7 @@
       </c>
       <c r="C768">
         <f>INDEX(Residents[], MATCH(B768,Residents[fullName], 0), 1)</f>
-        <v>2817</v>
+        <v>3085</v>
       </c>
       <c r="D768" t="s">
         <v>18</v>
@@ -15841,7 +15841,7 @@
       </c>
       <c r="C769">
         <f>INDEX(Residents[], MATCH(B769,Residents[fullName], 0), 1)</f>
-        <v>2818</v>
+        <v>3086</v>
       </c>
       <c r="D769" t="s">
         <v>4</v>
@@ -15860,7 +15860,7 @@
       </c>
       <c r="C770">
         <f>INDEX(Residents[], MATCH(B770,Residents[fullName], 0), 1)</f>
-        <v>2818</v>
+        <v>3086</v>
       </c>
       <c r="D770" t="s">
         <v>5</v>
@@ -15879,7 +15879,7 @@
       </c>
       <c r="C771">
         <f>INDEX(Residents[], MATCH(B771,Residents[fullName], 0), 1)</f>
-        <v>2818</v>
+        <v>3086</v>
       </c>
       <c r="D771" t="s">
         <v>6</v>
@@ -15898,7 +15898,7 @@
       </c>
       <c r="C772">
         <f>INDEX(Residents[], MATCH(B772,Residents[fullName], 0), 1)</f>
-        <v>2818</v>
+        <v>3086</v>
       </c>
       <c r="D772" t="s">
         <v>7</v>
@@ -15917,7 +15917,7 @@
       </c>
       <c r="C773">
         <f>INDEX(Residents[], MATCH(B773,Residents[fullName], 0), 1)</f>
-        <v>2818</v>
+        <v>3086</v>
       </c>
       <c r="D773" t="s">
         <v>9</v>
@@ -15936,7 +15936,7 @@
       </c>
       <c r="C774">
         <f>INDEX(Residents[], MATCH(B774,Residents[fullName], 0), 1)</f>
-        <v>2818</v>
+        <v>3086</v>
       </c>
       <c r="D774" t="s">
         <v>11</v>
@@ -15955,7 +15955,7 @@
       </c>
       <c r="C775">
         <f>INDEX(Residents[], MATCH(B775,Residents[fullName], 0), 1)</f>
-        <v>2818</v>
+        <v>3086</v>
       </c>
       <c r="D775" t="s">
         <v>12</v>
@@ -15974,7 +15974,7 @@
       </c>
       <c r="C776">
         <f>INDEX(Residents[], MATCH(B776,Residents[fullName], 0), 1)</f>
-        <v>2818</v>
+        <v>3086</v>
       </c>
       <c r="D776" t="s">
         <v>13</v>
@@ -15993,7 +15993,7 @@
       </c>
       <c r="C777">
         <f>INDEX(Residents[], MATCH(B777,Residents[fullName], 0), 1)</f>
-        <v>2818</v>
+        <v>3086</v>
       </c>
       <c r="D777" t="s">
         <v>14</v>
@@ -16012,7 +16012,7 @@
       </c>
       <c r="C778">
         <f>INDEX(Residents[], MATCH(B778,Residents[fullName], 0), 1)</f>
-        <v>2818</v>
+        <v>3086</v>
       </c>
       <c r="D778" t="s">
         <v>15</v>
@@ -16031,7 +16031,7 @@
       </c>
       <c r="C779">
         <f>INDEX(Residents[], MATCH(B779,Residents[fullName], 0), 1)</f>
-        <v>2818</v>
+        <v>3086</v>
       </c>
       <c r="D779" t="s">
         <v>16</v>
@@ -16050,7 +16050,7 @@
       </c>
       <c r="C780">
         <f>INDEX(Residents[], MATCH(B780,Residents[fullName], 0), 1)</f>
-        <v>2818</v>
+        <v>3086</v>
       </c>
       <c r="D780" t="s">
         <v>17</v>
@@ -16069,7 +16069,7 @@
       </c>
       <c r="C781">
         <f>INDEX(Residents[], MATCH(B781,Residents[fullName], 0), 1)</f>
-        <v>2818</v>
+        <v>3086</v>
       </c>
       <c r="D781" t="s">
         <v>18</v>
@@ -16088,7 +16088,7 @@
       </c>
       <c r="C782">
         <f>INDEX(Residents[], MATCH(B782,Residents[fullName], 0), 1)</f>
-        <v>2819</v>
+        <v>3087</v>
       </c>
       <c r="D782" t="s">
         <v>4</v>
@@ -16107,7 +16107,7 @@
       </c>
       <c r="C783">
         <f>INDEX(Residents[], MATCH(B783,Residents[fullName], 0), 1)</f>
-        <v>2819</v>
+        <v>3087</v>
       </c>
       <c r="D783" t="s">
         <v>5</v>
@@ -16126,7 +16126,7 @@
       </c>
       <c r="C784">
         <f>INDEX(Residents[], MATCH(B784,Residents[fullName], 0), 1)</f>
-        <v>2819</v>
+        <v>3087</v>
       </c>
       <c r="D784" t="s">
         <v>6</v>
@@ -16145,7 +16145,7 @@
       </c>
       <c r="C785">
         <f>INDEX(Residents[], MATCH(B785,Residents[fullName], 0), 1)</f>
-        <v>2819</v>
+        <v>3087</v>
       </c>
       <c r="D785" t="s">
         <v>7</v>
@@ -16164,7 +16164,7 @@
       </c>
       <c r="C786">
         <f>INDEX(Residents[], MATCH(B786,Residents[fullName], 0), 1)</f>
-        <v>2819</v>
+        <v>3087</v>
       </c>
       <c r="D786" t="s">
         <v>9</v>
@@ -16183,7 +16183,7 @@
       </c>
       <c r="C787">
         <f>INDEX(Residents[], MATCH(B787,Residents[fullName], 0), 1)</f>
-        <v>2819</v>
+        <v>3087</v>
       </c>
       <c r="D787" t="s">
         <v>11</v>
@@ -16202,7 +16202,7 @@
       </c>
       <c r="C788">
         <f>INDEX(Residents[], MATCH(B788,Residents[fullName], 0), 1)</f>
-        <v>2819</v>
+        <v>3087</v>
       </c>
       <c r="D788" t="s">
         <v>12</v>
@@ -16221,7 +16221,7 @@
       </c>
       <c r="C789">
         <f>INDEX(Residents[], MATCH(B789,Residents[fullName], 0), 1)</f>
-        <v>2819</v>
+        <v>3087</v>
       </c>
       <c r="D789" t="s">
         <v>13</v>
@@ -16240,7 +16240,7 @@
       </c>
       <c r="C790">
         <f>INDEX(Residents[], MATCH(B790,Residents[fullName], 0), 1)</f>
-        <v>2819</v>
+        <v>3087</v>
       </c>
       <c r="D790" t="s">
         <v>14</v>
@@ -16259,7 +16259,7 @@
       </c>
       <c r="C791">
         <f>INDEX(Residents[], MATCH(B791,Residents[fullName], 0), 1)</f>
-        <v>2819</v>
+        <v>3087</v>
       </c>
       <c r="D791" t="s">
         <v>15</v>
@@ -16278,7 +16278,7 @@
       </c>
       <c r="C792">
         <f>INDEX(Residents[], MATCH(B792,Residents[fullName], 0), 1)</f>
-        <v>2819</v>
+        <v>3087</v>
       </c>
       <c r="D792" t="s">
         <v>16</v>
@@ -16297,7 +16297,7 @@
       </c>
       <c r="C793">
         <f>INDEX(Residents[], MATCH(B793,Residents[fullName], 0), 1)</f>
-        <v>2819</v>
+        <v>3087</v>
       </c>
       <c r="D793" t="s">
         <v>17</v>
@@ -16316,7 +16316,7 @@
       </c>
       <c r="C794">
         <f>INDEX(Residents[], MATCH(B794,Residents[fullName], 0), 1)</f>
-        <v>2819</v>
+        <v>3087</v>
       </c>
       <c r="D794" t="s">
         <v>18</v>
@@ -16335,7 +16335,7 @@
       </c>
       <c r="C795" s="4">
         <f>INDEX(Residents[], MATCH(B795,Residents[fullName], 0), 1)</f>
-        <v>2821</v>
+        <v>3148</v>
       </c>
       <c r="D795" t="s">
         <v>4</v>
@@ -16354,7 +16354,7 @@
       </c>
       <c r="C796" s="4">
         <f>INDEX(Residents[], MATCH(B796,Residents[fullName], 0), 1)</f>
-        <v>2821</v>
+        <v>3148</v>
       </c>
       <c r="D796" t="s">
         <v>5</v>
@@ -16373,7 +16373,7 @@
       </c>
       <c r="C797" s="4">
         <f>INDEX(Residents[], MATCH(B797,Residents[fullName], 0), 1)</f>
-        <v>2821</v>
+        <v>3148</v>
       </c>
       <c r="D797" t="s">
         <v>6</v>
@@ -16392,7 +16392,7 @@
       </c>
       <c r="C798" s="4">
         <f>INDEX(Residents[], MATCH(B798,Residents[fullName], 0), 1)</f>
-        <v>2821</v>
+        <v>3148</v>
       </c>
       <c r="D798" t="s">
         <v>7</v>
@@ -16411,7 +16411,7 @@
       </c>
       <c r="C799" s="4">
         <f>INDEX(Residents[], MATCH(B799,Residents[fullName], 0), 1)</f>
-        <v>2821</v>
+        <v>3148</v>
       </c>
       <c r="D799" t="s">
         <v>9</v>
@@ -16430,7 +16430,7 @@
       </c>
       <c r="C800" s="4">
         <f>INDEX(Residents[], MATCH(B800,Residents[fullName], 0), 1)</f>
-        <v>2821</v>
+        <v>3148</v>
       </c>
       <c r="D800" t="s">
         <v>11</v>
@@ -16449,7 +16449,7 @@
       </c>
       <c r="C801" s="4">
         <f>INDEX(Residents[], MATCH(B801,Residents[fullName], 0), 1)</f>
-        <v>2821</v>
+        <v>3148</v>
       </c>
       <c r="D801" t="s">
         <v>12</v>
@@ -16468,7 +16468,7 @@
       </c>
       <c r="C802" s="4">
         <f>INDEX(Residents[], MATCH(B802,Residents[fullName], 0), 1)</f>
-        <v>2821</v>
+        <v>3148</v>
       </c>
       <c r="D802" t="s">
         <v>13</v>
@@ -16487,7 +16487,7 @@
       </c>
       <c r="C803" s="4">
         <f>INDEX(Residents[], MATCH(B803,Residents[fullName], 0), 1)</f>
-        <v>2821</v>
+        <v>3148</v>
       </c>
       <c r="D803" t="s">
         <v>14</v>
@@ -16506,7 +16506,7 @@
       </c>
       <c r="C804" s="4">
         <f>INDEX(Residents[], MATCH(B804,Residents[fullName], 0), 1)</f>
-        <v>2821</v>
+        <v>3148</v>
       </c>
       <c r="D804" t="s">
         <v>15</v>
@@ -16525,7 +16525,7 @@
       </c>
       <c r="C805" s="4">
         <f>INDEX(Residents[], MATCH(B805,Residents[fullName], 0), 1)</f>
-        <v>2821</v>
+        <v>3148</v>
       </c>
       <c r="D805" t="s">
         <v>16</v>
@@ -16544,7 +16544,7 @@
       </c>
       <c r="C806" s="4">
         <f>INDEX(Residents[], MATCH(B806,Residents[fullName], 0), 1)</f>
-        <v>2821</v>
+        <v>3148</v>
       </c>
       <c r="D806" t="s">
         <v>17</v>
@@ -16563,7 +16563,7 @@
       </c>
       <c r="C807" s="4">
         <f>INDEX(Residents[], MATCH(B807,Residents[fullName], 0), 1)</f>
-        <v>2821</v>
+        <v>3148</v>
       </c>
       <c r="D807" t="s">
         <v>18</v>
@@ -16582,7 +16582,7 @@
       </c>
       <c r="C808" s="4">
         <f>INDEX(Residents[], MATCH(B808,Residents[fullName], 0), 1)</f>
-        <v>2820</v>
+        <v>3114</v>
       </c>
       <c r="D808" t="s">
         <v>4</v>
@@ -16601,7 +16601,7 @@
       </c>
       <c r="C809" s="4">
         <f>INDEX(Residents[], MATCH(B809,Residents[fullName], 0), 1)</f>
-        <v>2820</v>
+        <v>3114</v>
       </c>
       <c r="D809" t="s">
         <v>5</v>
@@ -16620,7 +16620,7 @@
       </c>
       <c r="C810" s="4">
         <f>INDEX(Residents[], MATCH(B810,Residents[fullName], 0), 1)</f>
-        <v>2820</v>
+        <v>3114</v>
       </c>
       <c r="D810" t="s">
         <v>6</v>
@@ -16639,7 +16639,7 @@
       </c>
       <c r="C811" s="4">
         <f>INDEX(Residents[], MATCH(B811,Residents[fullName], 0), 1)</f>
-        <v>2820</v>
+        <v>3114</v>
       </c>
       <c r="D811" t="s">
         <v>7</v>
@@ -16658,7 +16658,7 @@
       </c>
       <c r="C812" s="4">
         <f>INDEX(Residents[], MATCH(B812,Residents[fullName], 0), 1)</f>
-        <v>2820</v>
+        <v>3114</v>
       </c>
       <c r="D812" t="s">
         <v>9</v>
@@ -16677,7 +16677,7 @@
       </c>
       <c r="C813" s="4">
         <f>INDEX(Residents[], MATCH(B813,Residents[fullName], 0), 1)</f>
-        <v>2820</v>
+        <v>3114</v>
       </c>
       <c r="D813" t="s">
         <v>11</v>
@@ -16696,7 +16696,7 @@
       </c>
       <c r="C814" s="4">
         <f>INDEX(Residents[], MATCH(B814,Residents[fullName], 0), 1)</f>
-        <v>2820</v>
+        <v>3114</v>
       </c>
       <c r="D814" t="s">
         <v>12</v>
@@ -16715,7 +16715,7 @@
       </c>
       <c r="C815" s="4">
         <f>INDEX(Residents[], MATCH(B815,Residents[fullName], 0), 1)</f>
-        <v>2820</v>
+        <v>3114</v>
       </c>
       <c r="D815" t="s">
         <v>13</v>
@@ -16734,7 +16734,7 @@
       </c>
       <c r="C816" s="4">
         <f>INDEX(Residents[], MATCH(B816,Residents[fullName], 0), 1)</f>
-        <v>2820</v>
+        <v>3114</v>
       </c>
       <c r="D816" t="s">
         <v>14</v>
@@ -16753,7 +16753,7 @@
       </c>
       <c r="C817" s="4">
         <f>INDEX(Residents[], MATCH(B817,Residents[fullName], 0), 1)</f>
-        <v>2820</v>
+        <v>3114</v>
       </c>
       <c r="D817" t="s">
         <v>15</v>
@@ -16772,7 +16772,7 @@
       </c>
       <c r="C818" s="4">
         <f>INDEX(Residents[], MATCH(B818,Residents[fullName], 0), 1)</f>
-        <v>2820</v>
+        <v>3114</v>
       </c>
       <c r="D818" t="s">
         <v>16</v>
@@ -16791,7 +16791,7 @@
       </c>
       <c r="C819" s="4">
         <f>INDEX(Residents[], MATCH(B819,Residents[fullName], 0), 1)</f>
-        <v>2820</v>
+        <v>3114</v>
       </c>
       <c r="D819" t="s">
         <v>17</v>
@@ -16810,7 +16810,7 @@
       </c>
       <c r="C820" s="4">
         <f>INDEX(Residents[], MATCH(B820,Residents[fullName], 0), 1)</f>
-        <v>2820</v>
+        <v>3114</v>
       </c>
       <c r="D820" t="s">
         <v>18</v>
@@ -17051,8 +17051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5CC31C-6869-47E7-A440-832340BE0ED2}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18075,8 +18075,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
-        <f>A46+1</f>
-        <v>2804</v>
+        <v>3072</v>
       </c>
       <c r="B47" t="s">
         <v>172</v>
@@ -18098,8 +18097,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
-        <f t="shared" ref="A48:A64" si="4">A47+1</f>
-        <v>2805</v>
+        <v>3073</v>
       </c>
       <c r="B48" t="s">
         <v>174</v>
@@ -18121,8 +18119,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
-        <f t="shared" si="4"/>
-        <v>2806</v>
+        <v>3074</v>
       </c>
       <c r="B49" t="s">
         <v>176</v>
@@ -18144,8 +18141,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
-        <f t="shared" si="4"/>
-        <v>2807</v>
+        <v>3075</v>
       </c>
       <c r="B50" t="s">
         <v>178</v>
@@ -18167,8 +18163,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
-        <f t="shared" si="4"/>
-        <v>2808</v>
+        <v>3076</v>
       </c>
       <c r="B51" t="s">
         <v>180</v>
@@ -18190,8 +18185,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
-        <f t="shared" si="4"/>
-        <v>2809</v>
+        <v>3077</v>
       </c>
       <c r="B52" t="s">
         <v>182</v>
@@ -18213,8 +18207,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
-        <f t="shared" si="4"/>
-        <v>2810</v>
+        <v>3078</v>
       </c>
       <c r="B53" t="s">
         <v>184</v>
@@ -18236,8 +18229,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
-        <f t="shared" si="4"/>
-        <v>2811</v>
+        <v>3079</v>
       </c>
       <c r="B54" t="s">
         <v>186</v>
@@ -18259,8 +18251,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
-        <f t="shared" si="4"/>
-        <v>2812</v>
+        <v>3080</v>
       </c>
       <c r="B55" t="s">
         <v>188</v>
@@ -18282,8 +18273,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
-        <f t="shared" si="4"/>
-        <v>2813</v>
+        <v>3081</v>
       </c>
       <c r="B56" t="s">
         <v>190</v>
@@ -18305,8 +18295,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
-        <f t="shared" si="4"/>
-        <v>2814</v>
+        <v>3082</v>
       </c>
       <c r="B57" t="s">
         <v>188</v>
@@ -18328,8 +18317,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
-        <f t="shared" si="4"/>
-        <v>2815</v>
+        <v>3083</v>
       </c>
       <c r="B58" t="s">
         <v>192</v>
@@ -18351,8 +18339,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
-        <f t="shared" si="4"/>
-        <v>2816</v>
+        <v>3084</v>
       </c>
       <c r="B59" t="s">
         <v>194</v>
@@ -18374,8 +18361,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
-        <f t="shared" si="4"/>
-        <v>2817</v>
+        <v>3085</v>
       </c>
       <c r="B60" t="s">
         <v>196</v>
@@ -18397,8 +18383,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
-        <f t="shared" si="4"/>
-        <v>2818</v>
+        <v>3086</v>
       </c>
       <c r="B61" t="s">
         <v>198</v>
@@ -18420,8 +18405,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
-        <f t="shared" si="4"/>
-        <v>2819</v>
+        <v>3087</v>
       </c>
       <c r="B62" t="s">
         <v>200</v>
@@ -18443,8 +18427,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
-        <f t="shared" si="4"/>
-        <v>2820</v>
+        <v>3114</v>
       </c>
       <c r="B63" t="s">
         <v>235</v>
@@ -18453,11 +18436,11 @@
         <v>234</v>
       </c>
       <c r="D63" s="4" t="str">
-        <f t="shared" ref="D63:D64" si="5">_xlfn.CONCAT(C63, ", ", B63)</f>
+        <f t="shared" ref="D63:D64" si="4">_xlfn.CONCAT(C63, ", ", B63)</f>
         <v>Sooryakumar, Dhriti</v>
       </c>
       <c r="E63" s="4" t="str">
-        <f t="shared" ref="E63:E64" si="6">CONCATENATE(LEFT(B63, 1), " ", C63)</f>
+        <f t="shared" ref="E63:E64" si="5">CONCATENATE(LEFT(B63, 1), " ", C63)</f>
         <v>D Sooryakumar</v>
       </c>
       <c r="F63">
@@ -18466,8 +18449,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
-        <f t="shared" si="4"/>
-        <v>2821</v>
+        <v>3148</v>
       </c>
       <c r="B64" t="s">
         <v>132</v>
@@ -18476,11 +18458,11 @@
         <v>236</v>
       </c>
       <c r="D64" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Mroz, John</v>
+      </c>
+      <c r="E64" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>Mroz, John</v>
-      </c>
-      <c r="E64" s="4" t="str">
-        <f t="shared" si="6"/>
         <v>J Mroz</v>
       </c>
       <c r="F64">

</xml_diff>

<commit_message>
fix: switching order of half block rotation
</commit_message>
<xml_diff>
--- a/data/residoodle_db.xlsx
+++ b/data/residoodle_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackie.fortinflefil/PERSONAL/code/residoodle/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C2BA9B-62AE-3C47-BBDF-897BC870CE5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0785BBAD-B4AA-9146-AFF7-E512C76945F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" activeTab="2" xr2:uid="{83F12362-36DA-4988-9448-F131A11196ED}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{83F12362-36DA-4988-9448-F131A11196ED}"/>
   </bookViews>
   <sheets>
     <sheet name="ResidentBlockSchedule" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2598" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2598" uniqueCount="240">
   <si>
     <t>Resident</t>
   </si>
@@ -766,6 +766,9 @@
   </si>
   <si>
     <t>Sooryakumar, Dhriti</t>
+  </si>
+  <si>
+    <t>H Trauma/ED</t>
   </si>
 </sst>
 </file>
@@ -1230,8 +1233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF91F7E-A94A-4218-9434-30BEAB935884}">
   <dimension ref="A1:E820"/>
   <sheetViews>
-    <sheetView topLeftCell="A750" workbookViewId="0">
-      <selection activeCell="E819" sqref="E819"/>
+    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
+      <selection activeCell="F331" sqref="F331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7392,7 +7395,7 @@
         <v>16</v>
       </c>
       <c r="E324" t="s">
-        <v>58</v>
+        <v>239</v>
       </c>
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.2">
@@ -17051,8 +17054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5CC31C-6869-47E7-A440-832340BE0ED2}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>